<commit_message>
Add test cases for EmailReminderChangeType and EmailReminderSendOption.
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSMTGS/MS-OXWSMTGS_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSMTGS/MS-OXWSMTGS_RequirementSpecification.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EWS&amp;EAS\MS-OXWSMTGS\MS-OXWSMTGS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EWS&amp;EAS\MS-OXWSMTGS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EAD70966-CC50-4F70-B85F-EBA73F7E7597}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F3CDB4-0439-4559-A702-D0EA65E661C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10321,6 +10321,30 @@
     <xf numFmtId="49" fontId="7" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -10353,30 +10377,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -14273,16 +14273,16 @@
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" ht="21">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="87"/>
-      <c r="C4" s="87"/>
-      <c r="D4" s="87"/>
-      <c r="E4" s="87"/>
-      <c r="F4" s="87"/>
-      <c r="G4" s="87"/>
-      <c r="H4" s="87"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
       <c r="I4" s="25"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -14294,13 +14294,13 @@
       <c r="B5" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="88"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="89"/>
-      <c r="H5" s="89"/>
-      <c r="I5" s="90"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="78"/>
+      <c r="I5" s="79"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
@@ -14308,16 +14308,16 @@
       <c r="A6" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="91" t="s">
+      <c r="B6" s="80" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="89"/>
-      <c r="D6" s="89"/>
-      <c r="E6" s="89"/>
-      <c r="F6" s="89"/>
-      <c r="G6" s="89"/>
-      <c r="H6" s="89"/>
-      <c r="I6" s="90"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="78"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="78"/>
+      <c r="H6" s="78"/>
+      <c r="I6" s="79"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
@@ -14325,16 +14325,16 @@
       <c r="A7" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="92" t="s">
+      <c r="B7" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="93"/>
-      <c r="D7" s="93"/>
-      <c r="E7" s="93"/>
-      <c r="F7" s="93"/>
-      <c r="G7" s="93"/>
-      <c r="H7" s="93"/>
-      <c r="I7" s="94"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="82"/>
+      <c r="I7" s="83"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
@@ -14342,16 +14342,16 @@
       <c r="A8" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="92" t="s">
+      <c r="B8" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="93"/>
-      <c r="D8" s="93"/>
-      <c r="E8" s="93"/>
-      <c r="F8" s="93"/>
-      <c r="G8" s="93"/>
-      <c r="H8" s="93"/>
-      <c r="I8" s="94"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="82"/>
+      <c r="E8" s="82"/>
+      <c r="F8" s="82"/>
+      <c r="G8" s="82"/>
+      <c r="H8" s="82"/>
+      <c r="I8" s="83"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
     </row>
@@ -14359,16 +14359,16 @@
       <c r="A9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="79" t="s">
+      <c r="B9" s="87" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="80"/>
-      <c r="D9" s="80"/>
-      <c r="E9" s="80"/>
-      <c r="F9" s="80"/>
-      <c r="G9" s="80"/>
-      <c r="H9" s="80"/>
-      <c r="I9" s="81"/>
+      <c r="C9" s="88"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="88"/>
+      <c r="F9" s="88"/>
+      <c r="G9" s="88"/>
+      <c r="H9" s="88"/>
+      <c r="I9" s="89"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
     </row>
@@ -14376,16 +14376,16 @@
       <c r="A10" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="79" t="s">
+      <c r="B10" s="87" t="s">
         <v>1649</v>
       </c>
-      <c r="C10" s="80"/>
-      <c r="D10" s="80"/>
-      <c r="E10" s="80"/>
-      <c r="F10" s="80"/>
-      <c r="G10" s="80"/>
-      <c r="H10" s="80"/>
-      <c r="I10" s="81"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="88"/>
+      <c r="E10" s="88"/>
+      <c r="F10" s="88"/>
+      <c r="G10" s="88"/>
+      <c r="H10" s="88"/>
+      <c r="I10" s="89"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
     </row>
@@ -14393,16 +14393,16 @@
       <c r="A11" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="82" t="s">
+      <c r="B11" s="90" t="s">
         <v>1650</v>
       </c>
-      <c r="C11" s="83"/>
-      <c r="D11" s="77"/>
-      <c r="E11" s="77"/>
-      <c r="F11" s="77"/>
-      <c r="G11" s="77"/>
-      <c r="H11" s="77"/>
-      <c r="I11" s="78"/>
+      <c r="C11" s="91"/>
+      <c r="D11" s="85"/>
+      <c r="E11" s="85"/>
+      <c r="F11" s="85"/>
+      <c r="G11" s="85"/>
+      <c r="H11" s="85"/>
+      <c r="I11" s="86"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
     </row>
@@ -14486,16 +14486,16 @@
       <c r="A16" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="84" t="s">
+      <c r="B16" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="85"/>
-      <c r="D16" s="77"/>
-      <c r="E16" s="77"/>
-      <c r="F16" s="77"/>
-      <c r="G16" s="77"/>
-      <c r="H16" s="77"/>
-      <c r="I16" s="78"/>
+      <c r="C16" s="93"/>
+      <c r="D16" s="85"/>
+      <c r="E16" s="85"/>
+      <c r="F16" s="85"/>
+      <c r="G16" s="85"/>
+      <c r="H16" s="85"/>
+      <c r="I16" s="86"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
     </row>
@@ -14503,16 +14503,16 @@
       <c r="A17" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="86" t="s">
+      <c r="B17" s="94" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="77"/>
-      <c r="D17" s="77"/>
-      <c r="E17" s="77"/>
-      <c r="F17" s="77"/>
-      <c r="G17" s="77"/>
-      <c r="H17" s="77"/>
-      <c r="I17" s="78"/>
+      <c r="C17" s="85"/>
+      <c r="D17" s="85"/>
+      <c r="E17" s="85"/>
+      <c r="F17" s="85"/>
+      <c r="G17" s="85"/>
+      <c r="H17" s="85"/>
+      <c r="I17" s="86"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
     </row>
@@ -14520,16 +14520,16 @@
       <c r="A18" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="76" t="s">
+      <c r="B18" s="84" t="s">
         <v>1651</v>
       </c>
-      <c r="C18" s="77"/>
-      <c r="D18" s="77"/>
-      <c r="E18" s="77"/>
-      <c r="F18" s="77"/>
-      <c r="G18" s="77"/>
-      <c r="H18" s="77"/>
-      <c r="I18" s="78"/>
+      <c r="C18" s="85"/>
+      <c r="D18" s="85"/>
+      <c r="E18" s="85"/>
+      <c r="F18" s="85"/>
+      <c r="G18" s="85"/>
+      <c r="H18" s="85"/>
+      <c r="I18" s="86"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="M18" s="4"/>
@@ -30026,7 +30026,7 @@
         <v>15</v>
       </c>
       <c r="H629" s="39" t="s">
-        <v>2574</v>
+        <v>2573</v>
       </c>
       <c r="I629" s="41"/>
     </row>
@@ -30051,7 +30051,7 @@
         <v>15</v>
       </c>
       <c r="H630" s="39" t="s">
-        <v>2574</v>
+        <v>2573</v>
       </c>
       <c r="I630" s="41"/>
     </row>
@@ -30076,7 +30076,7 @@
         <v>15</v>
       </c>
       <c r="H631" s="39" t="s">
-        <v>2574</v>
+        <v>2573</v>
       </c>
       <c r="I631" s="41"/>
     </row>
@@ -30101,7 +30101,7 @@
         <v>15</v>
       </c>
       <c r="H632" s="39" t="s">
-        <v>2574</v>
+        <v>2573</v>
       </c>
       <c r="I632" s="41"/>
     </row>
@@ -30228,7 +30228,7 @@
         <v>15</v>
       </c>
       <c r="H637" s="39" t="s">
-        <v>2574</v>
+        <v>2573</v>
       </c>
       <c r="I637" s="41"/>
     </row>
@@ -30253,7 +30253,7 @@
         <v>15</v>
       </c>
       <c r="H638" s="39" t="s">
-        <v>18</v>
+        <v>2573</v>
       </c>
       <c r="I638" s="41"/>
     </row>
@@ -44548,17 +44548,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B8:I8"/>
     <mergeCell ref="B18:I18"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B16:I16"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B8:I8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1050:I1050 A1117:I1117 A1119:I1119 A1125:I1125 A1129:I1129 A1131:I1131 A1133:I1133 A1137:I1143 E133:H133 E148:H148 E198:H198 E351:H351 E1030:I1030 E1036:I1048 E1080:I1080 E1092:I1092 E131:I132 E130:H130 E349:I350 E348:H348 E211:H212 E341:I347 E433:I460 E431:H432 E463:I469 E461:H462 E470:H470 E1155:I1190 E1154:H1154 E1144:I1153 E1029:H1029 E1031:H1035 E1079:H1079 E1081:H1083 E1091:H1091 E1093:H1093 E1101:H1101 C1049:E1049 C1051:E1051 C1116:E1116 C1118:E1118 C1120:E1120 C1126:E1128 C1130:E1130 C1132:E1132 E332:H334 E134:I147 A1026:D1048 E199:I208 E1028:I1028 E1026:H1027 E210:I210 E209:H209 E325:I331 E324:H324 E430:I430 E429:H429 E471:I484 E107:I129 E106:H106 I81 A278:I278 H279:I279 E336:H340 A81 A279 A335 E1078:I1078 A1076:I1077 A1144:D1190 E1071:H1071 E1072:I1075 A20:I80 A82:I86 E87:I105 E149:I197 A298:D334 E298:I323 A795:B795 D795:I795 A847:B847 D847:I847 A1022:B1025 D1022:I1025 A1052:D1075 E1052:I1070 E1084:I1090 E1094:I1100 E1102:I1109 A1078:D1109 A1110:I1110 I1112 C1111:E1111 H1111 A1112:H1114 A1115:I1115 H1120 A1121:A1124 C1121:H1124 C1134:H1136 A796:I846 A87:D277 E213:I277 A280:I297 A336:D484 E352:I428 A485:I794 A848:I869 A872:I1012 A870:C871 E870:I871">
@@ -46748,12 +46748,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -46802,6 +46796,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -46812,20 +46812,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -46840,6 +46826,20 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Update MS-OXWSMTGS RS and test case to keep consistent.
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSMTGS/MS-OXWSMTGS_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSMTGS/MS-OXWSMTGS_RequirementSpecification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EWS&amp;EAS\MS-OXWSMTGS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4148ACCB-AFC4-4EA9-B025-52730CB40832}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5CBCD3-7D7C-47B1-880C-9E1BA305C78D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="12900" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8565" uniqueCount="2681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8565" uniqueCount="2682">
   <si>
     <t>Req ID</t>
   </si>
@@ -8790,9 +8790,6 @@
     <t>MS-OXWSMTGS_R2182</t>
   </si>
   <si>
-    <t>MS-OXWSMTGS_R2183</t>
-  </si>
-  <si>
     <t>MS-OXWSMTGS_R203:i</t>
   </si>
   <si>
@@ -8910,15 +8907,9 @@
     <t>[In Appendix C: Product Behavior] Implementation does not support the EndTimeZone element. (&lt;40&gt; Section 2.2.4.17:  Exchange 2007 does not support the EndTimeZone element.)</t>
   </si>
   <si>
-    <t>MS-OXWSMTGS_R2190</t>
-  </si>
-  <si>
     <t>MS-OXWSMTGS_R2191</t>
   </si>
   <si>
-    <t>[In Appendix C: Product Behavior] Implementation does support ConferenceType in MeetingRequestMessageType. (&lt;41&gt; Section 2.2.4.17:  Exchange 2007, Exchange 2010, and Exchange 2013 support the ConferenceType element. The ConferenceType element is obsolete in Exchange 2016 and Exchange 2019.)</t>
-  </si>
-  <si>
     <t>Verified by derived requirement: MS-OXWSMTGS_R2190.</t>
   </si>
   <si>
@@ -8932,9 +8923,6 @@
   </si>
   <si>
     <t>[In Appendix C: Product Behavior] Implementation does not support the EndWallClock element. (&lt;44&gt; Section 2.2.4.17:  Exchange 2007 and Exchange 2010 do not support the EndWallClock element.)</t>
-  </si>
-  <si>
-    <t>[In Appendix C: Product Behavior] Implementation does support ConferenceType in CalendarItemType. (&lt;16&gt; Section 2.2.4.6:  Exchange 2007, Exchange 2010, and Exchange 2013 support the ConferenceType element. )</t>
   </si>
   <si>
     <t>Verified by derived requirement: MS-OXWSMTGS_R2187.</t>
@@ -9857,6 +9845,26 @@
   </si>
   <si>
     <t>[In Appendix C: Product Behavior] Implementation does use the value "WorkingElsewhere" which specifies the status as working outside the office. (Exchange 2013 and above follow this behavior.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior]Implementation does support TimeZone element if the meeting is not associated with a recurring calendar item. (Exchange 2007, Exchange 2010 and Exchange 2013 follow this behavior.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MS-OXWSMTGS_R3311</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MS-OXWSMTGS_R3541</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Implementation does support ConferenceType in CalendarItemType. (&lt;16&gt; Section 2.2.4.6:  Exchange 2007, Exchange 2010, and Exchange 2013 support the ConferenceType element. )</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Implementation does support ConferenceType in MeetingRequestMessageType. (&lt;41&gt; Section 2.2.4.17:  Exchange 2007, Exchange 2010, and Exchange 2013 support the ConferenceType element. The ConferenceType element is obsolete in Exchange 2016 and Exchange 2019.)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -10239,30 +10247,6 @@
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -10295,6 +10279,30 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -14179,16 +14187,16 @@
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" ht="21">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
       <c r="I4" s="25"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -14200,13 +14208,13 @@
       <c r="B5" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="54"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="65"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
@@ -14214,16 +14222,16 @@
       <c r="A6" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53"/>
-      <c r="H6" s="53"/>
-      <c r="I6" s="54"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="64"/>
+      <c r="I6" s="65"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
@@ -14231,16 +14239,16 @@
       <c r="A7" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="58"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="68"/>
+      <c r="H7" s="68"/>
+      <c r="I7" s="69"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
@@ -14248,16 +14256,16 @@
       <c r="A8" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="56" t="s">
+      <c r="B8" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="58"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="68"/>
+      <c r="I8" s="69"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
     </row>
@@ -14265,16 +14273,16 @@
       <c r="A9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="62" t="s">
+      <c r="B9" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="63"/>
-      <c r="I9" s="64"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="56"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
     </row>
@@ -14282,16 +14290,16 @@
       <c r="A10" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="62" t="s">
+      <c r="B10" s="54" t="s">
         <v>1648</v>
       </c>
-      <c r="C10" s="63"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="63"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="64"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="56"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
     </row>
@@ -14299,16 +14307,16 @@
       <c r="A11" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="65" t="s">
+      <c r="B11" s="57" t="s">
         <v>1649</v>
       </c>
-      <c r="C11" s="66"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="61"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="53"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
     </row>
@@ -14392,16 +14400,16 @@
       <c r="A16" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="67" t="s">
+      <c r="B16" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="68"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="60"/>
-      <c r="G16" s="60"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="61"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="53"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
     </row>
@@ -14409,16 +14417,16 @@
       <c r="A17" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="69" t="s">
+      <c r="B17" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="60"/>
-      <c r="D17" s="60"/>
-      <c r="E17" s="60"/>
-      <c r="F17" s="60"/>
-      <c r="G17" s="60"/>
-      <c r="H17" s="60"/>
-      <c r="I17" s="61"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="53"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
     </row>
@@ -14426,16 +14434,16 @@
       <c r="A18" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="51" t="s">
         <v>1650</v>
       </c>
-      <c r="C18" s="60"/>
-      <c r="D18" s="60"/>
-      <c r="E18" s="60"/>
-      <c r="F18" s="60"/>
-      <c r="G18" s="60"/>
-      <c r="H18" s="60"/>
-      <c r="I18" s="61"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="53"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="M18" s="4"/>
@@ -16059,7 +16067,7 @@
         <v>851</v>
       </c>
       <c r="C83" s="41" t="s">
-        <v>2580</v>
+        <v>2576</v>
       </c>
       <c r="D83" s="39"/>
       <c r="E83" s="39" t="s">
@@ -16072,7 +16080,7 @@
         <v>15</v>
       </c>
       <c r="H83" s="39" t="s">
-        <v>2570</v>
+        <v>2566</v>
       </c>
       <c r="I83" s="41"/>
     </row>
@@ -16109,7 +16117,7 @@
         <v>851</v>
       </c>
       <c r="C85" s="41" t="s">
-        <v>2571</v>
+        <v>2567</v>
       </c>
       <c r="D85" s="39"/>
       <c r="E85" s="39" t="s">
@@ -16122,7 +16130,7 @@
         <v>15</v>
       </c>
       <c r="H85" s="39" t="s">
-        <v>2570</v>
+        <v>2566</v>
       </c>
       <c r="I85" s="41"/>
     </row>
@@ -16144,7 +16152,7 @@
         <v>3</v>
       </c>
       <c r="G86" s="39" t="s">
-        <v>2581</v>
+        <v>2577</v>
       </c>
       <c r="H86" s="39" t="s">
         <v>18</v>
@@ -16409,7 +16417,7 @@
         <v>852</v>
       </c>
       <c r="C97" s="41" t="s">
-        <v>2673</v>
+        <v>2669</v>
       </c>
       <c r="D97" s="39"/>
       <c r="E97" s="39" t="s">
@@ -16601,7 +16609,7 @@
         <v>15</v>
       </c>
       <c r="H104" s="39" t="s">
-        <v>2564</v>
+        <v>2560</v>
       </c>
       <c r="I104" s="41"/>
     </row>
@@ -16765,7 +16773,7 @@
         <v>854</v>
       </c>
       <c r="C111" s="41" t="s">
-        <v>2566</v>
+        <v>2562</v>
       </c>
       <c r="D111" s="39"/>
       <c r="E111" s="39" t="s">
@@ -17260,7 +17268,7 @@
         <v>17</v>
       </c>
       <c r="I130" s="41" t="s">
-        <v>2526</v>
+        <v>2522</v>
       </c>
     </row>
     <row r="131" spans="1:9" ht="30">
@@ -18694,7 +18702,7 @@
         <v>17</v>
       </c>
       <c r="I186" s="41" t="s">
-        <v>2430</v>
+        <v>2429</v>
       </c>
     </row>
     <row r="187" spans="1:9">
@@ -19402,7 +19410,7 @@
         <v>20</v>
       </c>
       <c r="I214" s="41" t="s">
-        <v>2439</v>
+        <v>2438</v>
       </c>
     </row>
     <row r="215" spans="1:9" ht="30">
@@ -19665,7 +19673,7 @@
     </row>
     <row r="225" spans="1:9" s="37" customFormat="1">
       <c r="A225" s="39" t="s">
-        <v>2558</v>
+        <v>2554</v>
       </c>
       <c r="B225" s="40" t="s">
         <v>854</v>
@@ -19698,7 +19706,7 @@
         <v>854</v>
       </c>
       <c r="C226" s="41" t="s">
-        <v>2559</v>
+        <v>2555</v>
       </c>
       <c r="D226" s="48"/>
       <c r="E226" s="48" t="s">
@@ -19714,7 +19722,7 @@
         <v>17</v>
       </c>
       <c r="I226" s="41" t="s">
-        <v>2475</v>
+        <v>2471</v>
       </c>
     </row>
     <row r="227" spans="1:9">
@@ -20025,7 +20033,7 @@
         <v>15</v>
       </c>
       <c r="H238" s="39" t="s">
-        <v>2565</v>
+        <v>2561</v>
       </c>
       <c r="I238" s="49"/>
     </row>
@@ -20075,7 +20083,7 @@
         <v>15</v>
       </c>
       <c r="H240" s="39" t="s">
-        <v>2565</v>
+        <v>2561</v>
       </c>
       <c r="I240" s="49"/>
     </row>
@@ -20114,7 +20122,7 @@
         <v>854</v>
       </c>
       <c r="C242" s="41" t="s">
-        <v>2569</v>
+        <v>2565</v>
       </c>
       <c r="D242" s="48"/>
       <c r="E242" s="48" t="s">
@@ -20127,19 +20135,19 @@
         <v>15</v>
       </c>
       <c r="H242" s="39" t="s">
-        <v>2570</v>
+        <v>2566</v>
       </c>
       <c r="I242" s="49"/>
     </row>
     <row r="243" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A243" s="39" t="s">
-        <v>2568</v>
+        <v>2564</v>
       </c>
       <c r="B243" s="40" t="s">
-        <v>2567</v>
+        <v>2563</v>
       </c>
       <c r="C243" s="41" t="s">
-        <v>2584</v>
+        <v>2580</v>
       </c>
       <c r="D243" s="39"/>
       <c r="E243" s="48" t="s">
@@ -21041,7 +21049,7 @@
         <v>858</v>
       </c>
       <c r="C279" s="41" t="s">
-        <v>2572</v>
+        <v>2568</v>
       </c>
       <c r="D279" s="39"/>
       <c r="E279" s="39" t="s">
@@ -21054,7 +21062,7 @@
         <v>15</v>
       </c>
       <c r="H279" s="39" t="s">
-        <v>2570</v>
+        <v>2566</v>
       </c>
       <c r="I279" s="41"/>
     </row>
@@ -21066,7 +21074,7 @@
         <v>858</v>
       </c>
       <c r="C280" s="41" t="s">
-        <v>2573</v>
+        <v>2569</v>
       </c>
       <c r="D280" s="39"/>
       <c r="E280" s="39" t="s">
@@ -21079,7 +21087,7 @@
         <v>15</v>
       </c>
       <c r="H280" s="39" t="s">
-        <v>2570</v>
+        <v>2566</v>
       </c>
       <c r="I280" s="41"/>
     </row>
@@ -21091,7 +21099,7 @@
         <v>858</v>
       </c>
       <c r="C281" s="41" t="s">
-        <v>2585</v>
+        <v>2581</v>
       </c>
       <c r="D281" s="39"/>
       <c r="E281" s="39" t="s">
@@ -21104,7 +21112,7 @@
         <v>15</v>
       </c>
       <c r="H281" s="39" t="s">
-        <v>2564</v>
+        <v>2560</v>
       </c>
       <c r="I281" s="41"/>
     </row>
@@ -21116,7 +21124,7 @@
         <v>858</v>
       </c>
       <c r="C282" s="41" t="s">
-        <v>2574</v>
+        <v>2570</v>
       </c>
       <c r="D282" s="39"/>
       <c r="E282" s="39" t="s">
@@ -21129,7 +21137,7 @@
         <v>15</v>
       </c>
       <c r="H282" s="39" t="s">
-        <v>2570</v>
+        <v>2566</v>
       </c>
       <c r="I282" s="41"/>
     </row>
@@ -21141,7 +21149,7 @@
         <v>858</v>
       </c>
       <c r="C283" s="41" t="s">
-        <v>2586</v>
+        <v>2582</v>
       </c>
       <c r="D283" s="39"/>
       <c r="E283" s="39" t="s">
@@ -21154,7 +21162,7 @@
         <v>15</v>
       </c>
       <c r="H283" s="39" t="s">
-        <v>2564</v>
+        <v>2560</v>
       </c>
       <c r="I283" s="41"/>
     </row>
@@ -21166,7 +21174,7 @@
         <v>858</v>
       </c>
       <c r="C284" s="41" t="s">
-        <v>2575</v>
+        <v>2571</v>
       </c>
       <c r="D284" s="39"/>
       <c r="E284" s="39" t="s">
@@ -21179,7 +21187,7 @@
         <v>15</v>
       </c>
       <c r="H284" s="39" t="s">
-        <v>2570</v>
+        <v>2566</v>
       </c>
       <c r="I284" s="41"/>
     </row>
@@ -21191,7 +21199,7 @@
         <v>858</v>
       </c>
       <c r="C285" s="41" t="s">
-        <v>2587</v>
+        <v>2583</v>
       </c>
       <c r="D285" s="39"/>
       <c r="E285" s="39" t="s">
@@ -21204,7 +21212,7 @@
         <v>15</v>
       </c>
       <c r="H285" s="39" t="s">
-        <v>2564</v>
+        <v>2560</v>
       </c>
       <c r="I285" s="41"/>
     </row>
@@ -21216,7 +21224,7 @@
         <v>858</v>
       </c>
       <c r="C286" s="41" t="s">
-        <v>2576</v>
+        <v>2572</v>
       </c>
       <c r="D286" s="39"/>
       <c r="E286" s="39" t="s">
@@ -21229,7 +21237,7 @@
         <v>15</v>
       </c>
       <c r="H286" s="39" t="s">
-        <v>2570</v>
+        <v>2566</v>
       </c>
       <c r="I286" s="41"/>
     </row>
@@ -21254,7 +21262,7 @@
         <v>15</v>
       </c>
       <c r="H287" s="39" t="s">
-        <v>2564</v>
+        <v>2560</v>
       </c>
       <c r="I287" s="41"/>
     </row>
@@ -21266,7 +21274,7 @@
         <v>858</v>
       </c>
       <c r="C288" s="41" t="s">
-        <v>2605</v>
+        <v>2601</v>
       </c>
       <c r="D288" s="39" t="s">
         <v>1884</v>
@@ -21281,7 +21289,7 @@
         <v>15</v>
       </c>
       <c r="H288" s="39" t="s">
-        <v>2564</v>
+        <v>2560</v>
       </c>
       <c r="I288" s="41"/>
     </row>
@@ -21293,7 +21301,7 @@
         <v>858</v>
       </c>
       <c r="C289" s="41" t="s">
-        <v>2588</v>
+        <v>2584</v>
       </c>
       <c r="D289" s="39" t="s">
         <v>1884</v>
@@ -21308,7 +21316,7 @@
         <v>15</v>
       </c>
       <c r="H289" s="39" t="s">
-        <v>2564</v>
+        <v>2560</v>
       </c>
       <c r="I289" s="41"/>
     </row>
@@ -21320,7 +21328,7 @@
         <v>858</v>
       </c>
       <c r="C290" s="41" t="s">
-        <v>2577</v>
+        <v>2573</v>
       </c>
       <c r="D290" s="39"/>
       <c r="E290" s="39" t="s">
@@ -21333,7 +21341,7 @@
         <v>15</v>
       </c>
       <c r="H290" s="39" t="s">
-        <v>2570</v>
+        <v>2566</v>
       </c>
       <c r="I290" s="41"/>
     </row>
@@ -21345,7 +21353,7 @@
         <v>858</v>
       </c>
       <c r="C291" s="41" t="s">
-        <v>2594</v>
+        <v>2590</v>
       </c>
       <c r="D291" s="39"/>
       <c r="E291" s="39" t="s">
@@ -21358,7 +21366,7 @@
         <v>15</v>
       </c>
       <c r="H291" s="39" t="s">
-        <v>2570</v>
+        <v>2566</v>
       </c>
       <c r="I291" s="41"/>
     </row>
@@ -21370,7 +21378,7 @@
         <v>858</v>
       </c>
       <c r="C292" s="41" t="s">
-        <v>2578</v>
+        <v>2574</v>
       </c>
       <c r="D292" s="48"/>
       <c r="E292" s="48" t="s">
@@ -21408,23 +21416,23 @@
         <v>15</v>
       </c>
       <c r="H293" s="39" t="s">
-        <v>2564</v>
+        <v>2560</v>
       </c>
       <c r="I293" s="49"/>
     </row>
     <row r="294" spans="1:9" s="37" customFormat="1">
       <c r="A294" s="39" t="s">
-        <v>2591</v>
+        <v>2587</v>
       </c>
       <c r="B294" s="40" t="s">
         <v>858</v>
       </c>
       <c r="C294" s="41" t="s">
+        <v>2585</v>
+      </c>
+      <c r="D294" s="39" t="s">
         <v>2589</v>
       </c>
-      <c r="D294" s="39" t="s">
-        <v>2593</v>
-      </c>
       <c r="E294" s="48" t="s">
         <v>19</v>
       </c>
@@ -21435,22 +21443,22 @@
         <v>15</v>
       </c>
       <c r="H294" s="39" t="s">
-        <v>2565</v>
+        <v>2561</v>
       </c>
       <c r="I294" s="41"/>
     </row>
     <row r="295" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A295" s="39" t="s">
-        <v>2592</v>
+        <v>2588</v>
       </c>
       <c r="B295" s="40" t="s">
         <v>858</v>
       </c>
       <c r="C295" s="41" t="s">
-        <v>2590</v>
+        <v>2586</v>
       </c>
       <c r="D295" s="39" t="s">
-        <v>2593</v>
+        <v>2589</v>
       </c>
       <c r="E295" s="48" t="s">
         <v>19</v>
@@ -21462,7 +21470,7 @@
         <v>15</v>
       </c>
       <c r="H295" s="39" t="s">
-        <v>2564</v>
+        <v>2560</v>
       </c>
       <c r="I295" s="41"/>
     </row>
@@ -21474,7 +21482,7 @@
         <v>858</v>
       </c>
       <c r="C296" s="41" t="s">
-        <v>2579</v>
+        <v>2575</v>
       </c>
       <c r="D296" s="39"/>
       <c r="E296" s="39" t="s">
@@ -21487,7 +21495,7 @@
         <v>15</v>
       </c>
       <c r="H296" s="39" t="s">
-        <v>2570</v>
+        <v>2566</v>
       </c>
       <c r="I296" s="41"/>
     </row>
@@ -21499,7 +21507,7 @@
         <v>858</v>
       </c>
       <c r="C297" s="41" t="s">
-        <v>2672</v>
+        <v>2668</v>
       </c>
       <c r="D297" s="39"/>
       <c r="E297" s="39" t="s">
@@ -21512,7 +21520,7 @@
         <v>15</v>
       </c>
       <c r="H297" s="39" t="s">
-        <v>2570</v>
+        <v>2566</v>
       </c>
       <c r="I297" s="41"/>
     </row>
@@ -22814,7 +22822,7 @@
         <v>17</v>
       </c>
       <c r="I348" s="41" t="s">
-        <v>2527</v>
+        <v>2523</v>
       </c>
     </row>
     <row r="349" spans="1:9" ht="30">
@@ -23487,13 +23495,13 @@
     </row>
     <row r="375" spans="1:9">
       <c r="A375" s="39" t="s">
-        <v>2611</v>
+        <v>2607</v>
       </c>
       <c r="B375" s="40" t="s">
         <v>862</v>
       </c>
       <c r="C375" s="41" t="s">
-        <v>2612</v>
+        <v>2608</v>
       </c>
       <c r="D375" s="39"/>
       <c r="E375" s="39" t="s">
@@ -23506,7 +23514,7 @@
         <v>15</v>
       </c>
       <c r="H375" s="39" t="s">
-        <v>2564</v>
+        <v>2560</v>
       </c>
       <c r="I375" s="41"/>
     </row>
@@ -24419,7 +24427,7 @@
         <v>17</v>
       </c>
       <c r="I411" s="41" t="s">
-        <v>2463</v>
+        <v>2462</v>
       </c>
     </row>
     <row r="412" spans="1:9">
@@ -25004,7 +25012,7 @@
         <v>20</v>
       </c>
       <c r="I434" s="41" t="s">
-        <v>2469</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="435" spans="1:9" ht="30">
@@ -29767,7 +29775,7 @@
         <v>873</v>
       </c>
       <c r="C623" s="41" t="s">
-        <v>2563</v>
+        <v>2559</v>
       </c>
       <c r="D623" s="39"/>
       <c r="E623" s="39" t="s">
@@ -29780,7 +29788,7 @@
         <v>15</v>
       </c>
       <c r="H623" s="39" t="s">
-        <v>2565</v>
+        <v>2561</v>
       </c>
       <c r="I623" s="41"/>
     </row>
@@ -29858,7 +29866,7 @@
         <v>17</v>
       </c>
       <c r="I626" s="41" t="s">
-        <v>2602</v>
+        <v>2598</v>
       </c>
     </row>
     <row r="627" spans="1:9" s="37" customFormat="1" ht="120">
@@ -29869,7 +29877,7 @@
         <v>874</v>
       </c>
       <c r="C627" s="41" t="s">
-        <v>2582</v>
+        <v>2578</v>
       </c>
       <c r="D627" s="39"/>
       <c r="E627" s="39" t="s">
@@ -29882,7 +29890,7 @@
         <v>15</v>
       </c>
       <c r="H627" s="39" t="s">
-        <v>2570</v>
+        <v>2566</v>
       </c>
       <c r="I627" s="41"/>
     </row>
@@ -29919,7 +29927,7 @@
         <v>874</v>
       </c>
       <c r="C629" s="41" t="s">
-        <v>2595</v>
+        <v>2591</v>
       </c>
       <c r="D629" s="39"/>
       <c r="E629" s="39" t="s">
@@ -29932,7 +29940,7 @@
         <v>15</v>
       </c>
       <c r="H629" s="39" t="s">
-        <v>2564</v>
+        <v>2560</v>
       </c>
       <c r="I629" s="41"/>
     </row>
@@ -29944,7 +29952,7 @@
         <v>874</v>
       </c>
       <c r="C630" s="41" t="s">
-        <v>2596</v>
+        <v>2592</v>
       </c>
       <c r="D630" s="39"/>
       <c r="E630" s="39" t="s">
@@ -29957,7 +29965,7 @@
         <v>15</v>
       </c>
       <c r="H630" s="39" t="s">
-        <v>2564</v>
+        <v>2560</v>
       </c>
       <c r="I630" s="41"/>
     </row>
@@ -29969,7 +29977,7 @@
         <v>874</v>
       </c>
       <c r="C631" s="41" t="s">
-        <v>2597</v>
+        <v>2593</v>
       </c>
       <c r="D631" s="39"/>
       <c r="E631" s="39" t="s">
@@ -29982,7 +29990,7 @@
         <v>15</v>
       </c>
       <c r="H631" s="39" t="s">
-        <v>2564</v>
+        <v>2560</v>
       </c>
       <c r="I631" s="41"/>
     </row>
@@ -29994,7 +30002,7 @@
         <v>874</v>
       </c>
       <c r="C632" s="41" t="s">
-        <v>2598</v>
+        <v>2594</v>
       </c>
       <c r="D632" s="39"/>
       <c r="E632" s="39" t="s">
@@ -30007,7 +30015,7 @@
         <v>15</v>
       </c>
       <c r="H632" s="39" t="s">
-        <v>2564</v>
+        <v>2560</v>
       </c>
       <c r="I632" s="41"/>
     </row>
@@ -30035,7 +30043,7 @@
         <v>17</v>
       </c>
       <c r="I633" s="41" t="s">
-        <v>2603</v>
+        <v>2599</v>
       </c>
     </row>
     <row r="634" spans="1:9" s="37" customFormat="1" ht="135">
@@ -30046,7 +30054,7 @@
         <v>875</v>
       </c>
       <c r="C634" s="41" t="s">
-        <v>2583</v>
+        <v>2579</v>
       </c>
       <c r="D634" s="39"/>
       <c r="E634" s="39" t="s">
@@ -30059,7 +30067,7 @@
         <v>15</v>
       </c>
       <c r="H634" s="39" t="s">
-        <v>2570</v>
+        <v>2566</v>
       </c>
       <c r="I634" s="41"/>
     </row>
@@ -30121,7 +30129,7 @@
         <v>875</v>
       </c>
       <c r="C637" s="41" t="s">
-        <v>2604</v>
+        <v>2600</v>
       </c>
       <c r="D637" s="39"/>
       <c r="E637" s="39" t="s">
@@ -30134,7 +30142,7 @@
         <v>15</v>
       </c>
       <c r="H637" s="39" t="s">
-        <v>2564</v>
+        <v>2560</v>
       </c>
       <c r="I637" s="41"/>
     </row>
@@ -30159,7 +30167,7 @@
         <v>15</v>
       </c>
       <c r="H638" s="39" t="s">
-        <v>2564</v>
+        <v>2560</v>
       </c>
       <c r="I638" s="41"/>
     </row>
@@ -30621,7 +30629,7 @@
         <v>877</v>
       </c>
       <c r="C657" s="41" t="s">
-        <v>2516</v>
+        <v>2512</v>
       </c>
       <c r="D657" s="39"/>
       <c r="E657" s="39" t="s">
@@ -30637,7 +30645,7 @@
         <v>17</v>
       </c>
       <c r="I657" s="41" t="s">
-        <v>2676</v>
+        <v>2672</v>
       </c>
     </row>
     <row r="658" spans="1:9" ht="150">
@@ -30814,7 +30822,7 @@
         <v>17</v>
       </c>
       <c r="I664" s="41" t="s">
-        <v>2556</v>
+        <v>2552</v>
       </c>
     </row>
     <row r="665" spans="1:9" s="37" customFormat="1" ht="30">
@@ -30891,7 +30899,7 @@
         <v>17</v>
       </c>
       <c r="I667" s="41" t="s">
-        <v>2557</v>
+        <v>2553</v>
       </c>
     </row>
     <row r="668" spans="1:9" s="38" customFormat="1">
@@ -32108,7 +32116,7 @@
         <v>885</v>
       </c>
       <c r="C716" s="41" t="s">
-        <v>2607</v>
+        <v>2603</v>
       </c>
       <c r="D716" s="39"/>
       <c r="E716" s="39" t="s">
@@ -32125,7 +32133,7 @@
       </c>
       <c r="I716" s="41"/>
       <c r="N716" s="37" t="s">
-        <v>2606</v>
+        <v>2602</v>
       </c>
     </row>
     <row r="717" spans="1:14" ht="30">
@@ -32815,7 +32823,7 @@
         <v>886</v>
       </c>
       <c r="C744" s="41" t="s">
-        <v>2613</v>
+        <v>2609</v>
       </c>
       <c r="D744" s="39"/>
       <c r="E744" s="39" t="s">
@@ -32856,7 +32864,7 @@
         <v>17</v>
       </c>
       <c r="I745" s="41" t="s">
-        <v>2616</v>
+        <v>2612</v>
       </c>
     </row>
     <row r="746" spans="1:9" ht="30">
@@ -33334,7 +33342,7 @@
         <v>15</v>
       </c>
       <c r="H764" s="39" t="s">
-        <v>2564</v>
+        <v>2560</v>
       </c>
       <c r="I764" s="41"/>
     </row>
@@ -33879,7 +33887,7 @@
         <v>890</v>
       </c>
       <c r="C786" s="41" t="s">
-        <v>2671</v>
+        <v>2667</v>
       </c>
       <c r="D786" s="39"/>
       <c r="E786" s="39" t="s">
@@ -33892,7 +33900,7 @@
         <v>15</v>
       </c>
       <c r="H786" s="39" t="s">
-        <v>2564</v>
+        <v>2560</v>
       </c>
       <c r="I786" s="41"/>
     </row>
@@ -33904,7 +33912,7 @@
         <v>890</v>
       </c>
       <c r="C787" s="41" t="s">
-        <v>2607</v>
+        <v>2603</v>
       </c>
       <c r="D787" s="39"/>
       <c r="E787" s="39" t="s">
@@ -33917,7 +33925,7 @@
         <v>15</v>
       </c>
       <c r="H787" s="39" t="s">
-        <v>2564</v>
+        <v>2560</v>
       </c>
       <c r="I787" s="41"/>
     </row>
@@ -33995,7 +34003,7 @@
         <v>17</v>
       </c>
       <c r="I790" s="41" t="s">
-        <v>2535</v>
+        <v>2531</v>
       </c>
     </row>
     <row r="791" spans="1:9" s="37" customFormat="1" ht="90">
@@ -34006,7 +34014,7 @@
         <v>891</v>
       </c>
       <c r="C791" s="41" t="s">
-        <v>2619</v>
+        <v>2615</v>
       </c>
       <c r="D791" s="48"/>
       <c r="E791" s="48" t="s">
@@ -34031,7 +34039,7 @@
         <v>891</v>
       </c>
       <c r="C792" s="41" t="s">
-        <v>2618</v>
+        <v>2614</v>
       </c>
       <c r="D792" s="48"/>
       <c r="E792" s="48" t="s">
@@ -34081,20 +34089,20 @@
         <v>892</v>
       </c>
       <c r="C794" s="41" t="s">
-        <v>2621</v>
+        <v>2617</v>
       </c>
       <c r="D794" s="48"/>
       <c r="E794" s="48" t="s">
         <v>19</v>
       </c>
       <c r="F794" s="39" t="s">
-        <v>2624</v>
+        <v>2620</v>
       </c>
       <c r="G794" s="48" t="s">
         <v>15</v>
       </c>
       <c r="H794" s="39" t="s">
-        <v>2565</v>
+        <v>2561</v>
       </c>
       <c r="I794" s="49"/>
     </row>
@@ -34106,7 +34114,7 @@
         <v>892</v>
       </c>
       <c r="C795" s="41" t="s">
-        <v>2622</v>
+        <v>2618</v>
       </c>
       <c r="D795" s="39"/>
       <c r="E795" s="39" t="s">
@@ -34119,7 +34127,7 @@
         <v>15</v>
       </c>
       <c r="H795" s="39" t="s">
-        <v>2570</v>
+        <v>2566</v>
       </c>
       <c r="I795" s="41"/>
     </row>
@@ -34138,7 +34146,7 @@
         <v>19</v>
       </c>
       <c r="F796" s="39" t="s">
-        <v>2624</v>
+        <v>2620</v>
       </c>
       <c r="G796" s="48" t="s">
         <v>15</v>
@@ -34163,13 +34171,13 @@
         <v>19</v>
       </c>
       <c r="F797" s="39" t="s">
-        <v>2624</v>
+        <v>2620</v>
       </c>
       <c r="G797" s="48" t="s">
         <v>15</v>
       </c>
       <c r="H797" s="39" t="s">
-        <v>2565</v>
+        <v>2561</v>
       </c>
       <c r="I797" s="49"/>
     </row>
@@ -34188,7 +34196,7 @@
         <v>19</v>
       </c>
       <c r="F798" s="39" t="s">
-        <v>2624</v>
+        <v>2620</v>
       </c>
       <c r="G798" s="48" t="s">
         <v>15</v>
@@ -34238,13 +34246,13 @@
         <v>19</v>
       </c>
       <c r="F800" s="39" t="s">
-        <v>2624</v>
+        <v>2620</v>
       </c>
       <c r="G800" s="48" t="s">
         <v>15</v>
       </c>
       <c r="H800" s="39" t="s">
-        <v>2565</v>
+        <v>2561</v>
       </c>
       <c r="I800" s="49"/>
     </row>
@@ -34263,7 +34271,7 @@
         <v>19</v>
       </c>
       <c r="F801" s="39" t="s">
-        <v>2624</v>
+        <v>2620</v>
       </c>
       <c r="G801" s="48" t="s">
         <v>15</v>
@@ -34288,13 +34296,13 @@
         <v>19</v>
       </c>
       <c r="F802" s="39" t="s">
-        <v>2624</v>
+        <v>2620</v>
       </c>
       <c r="G802" s="48" t="s">
         <v>15</v>
       </c>
       <c r="H802" s="39" t="s">
-        <v>2565</v>
+        <v>2561</v>
       </c>
       <c r="I802" s="49"/>
     </row>
@@ -34313,7 +34321,7 @@
         <v>19</v>
       </c>
       <c r="F803" s="39" t="s">
-        <v>2624</v>
+        <v>2620</v>
       </c>
       <c r="G803" s="48" t="s">
         <v>15</v>
@@ -34341,7 +34349,7 @@
         <v>3</v>
       </c>
       <c r="G804" s="39" t="s">
-        <v>2581</v>
+        <v>2577</v>
       </c>
       <c r="H804" s="48" t="s">
         <v>18</v>
@@ -34356,7 +34364,7 @@
         <v>2129</v>
       </c>
       <c r="C805" s="41" t="s">
-        <v>2623</v>
+        <v>2619</v>
       </c>
       <c r="D805" s="48"/>
       <c r="E805" s="48" t="s">
@@ -34391,7 +34399,7 @@
         <v>3</v>
       </c>
       <c r="G806" s="39" t="s">
-        <v>2581</v>
+        <v>2577</v>
       </c>
       <c r="H806" s="48" t="s">
         <v>18</v>
@@ -34431,7 +34439,7 @@
         <v>2129</v>
       </c>
       <c r="C808" s="41" t="s">
-        <v>2626</v>
+        <v>2622</v>
       </c>
       <c r="D808" s="48"/>
       <c r="E808" s="48" t="s">
@@ -34456,7 +34464,7 @@
         <v>2129</v>
       </c>
       <c r="C809" s="41" t="s">
-        <v>2627</v>
+        <v>2623</v>
       </c>
       <c r="D809" s="48"/>
       <c r="E809" s="48" t="s">
@@ -34469,7 +34477,7 @@
         <v>15</v>
       </c>
       <c r="H809" s="39" t="s">
-        <v>2570</v>
+        <v>2566</v>
       </c>
       <c r="I809" s="49"/>
     </row>
@@ -34481,7 +34489,7 @@
         <v>2129</v>
       </c>
       <c r="C810" s="41" t="s">
-        <v>2628</v>
+        <v>2624</v>
       </c>
       <c r="D810" s="48"/>
       <c r="E810" s="48" t="s">
@@ -34506,7 +34514,7 @@
         <v>2129</v>
       </c>
       <c r="C811" s="41" t="s">
-        <v>2629</v>
+        <v>2625</v>
       </c>
       <c r="D811" s="48"/>
       <c r="E811" s="48" t="s">
@@ -34519,7 +34527,7 @@
         <v>15</v>
       </c>
       <c r="H811" s="39" t="s">
-        <v>2570</v>
+        <v>2566</v>
       </c>
       <c r="I811" s="49"/>
     </row>
@@ -34531,7 +34539,7 @@
         <v>2129</v>
       </c>
       <c r="C812" s="41" t="s">
-        <v>2652</v>
+        <v>2648</v>
       </c>
       <c r="D812" s="48"/>
       <c r="E812" s="48" t="s">
@@ -34556,7 +34564,7 @@
         <v>2129</v>
       </c>
       <c r="C813" s="41" t="s">
-        <v>2653</v>
+        <v>2649</v>
       </c>
       <c r="D813" s="48"/>
       <c r="E813" s="48" t="s">
@@ -34594,7 +34602,7 @@
         <v>15</v>
       </c>
       <c r="H814" s="39" t="s">
-        <v>2565</v>
+        <v>2561</v>
       </c>
       <c r="I814" s="49"/>
     </row>
@@ -34619,7 +34627,7 @@
         <v>15</v>
       </c>
       <c r="H815" s="39" t="s">
-        <v>2565</v>
+        <v>2561</v>
       </c>
       <c r="I815" s="49"/>
     </row>
@@ -34656,20 +34664,20 @@
         <v>2153</v>
       </c>
       <c r="C817" s="41" t="s">
-        <v>2651</v>
+        <v>2647</v>
       </c>
       <c r="D817" s="48"/>
       <c r="E817" s="48" t="s">
         <v>19</v>
       </c>
       <c r="F817" s="39" t="s">
-        <v>2624</v>
+        <v>2620</v>
       </c>
       <c r="G817" s="48" t="s">
         <v>15</v>
       </c>
       <c r="H817" s="39" t="s">
-        <v>2565</v>
+        <v>2561</v>
       </c>
       <c r="I817" s="49"/>
     </row>
@@ -34681,7 +34689,7 @@
         <v>2153</v>
       </c>
       <c r="C818" s="41" t="s">
-        <v>2630</v>
+        <v>2626</v>
       </c>
       <c r="D818" s="48"/>
       <c r="E818" s="48" t="s">
@@ -34691,7 +34699,7 @@
         <v>3</v>
       </c>
       <c r="G818" s="39" t="s">
-        <v>2581</v>
+        <v>2577</v>
       </c>
       <c r="H818" s="48" t="s">
         <v>18</v>
@@ -34713,7 +34721,7 @@
         <v>19</v>
       </c>
       <c r="F819" s="39" t="s">
-        <v>2624</v>
+        <v>2620</v>
       </c>
       <c r="G819" s="48" t="s">
         <v>15</v>
@@ -34738,13 +34746,13 @@
         <v>19</v>
       </c>
       <c r="F820" s="39" t="s">
-        <v>2624</v>
+        <v>2620</v>
       </c>
       <c r="G820" s="48" t="s">
         <v>15</v>
       </c>
       <c r="H820" s="39" t="s">
-        <v>2565</v>
+        <v>2561</v>
       </c>
       <c r="I820" s="49"/>
     </row>
@@ -34756,7 +34764,7 @@
         <v>2158</v>
       </c>
       <c r="C821" s="41" t="s">
-        <v>2632</v>
+        <v>2628</v>
       </c>
       <c r="D821" s="48"/>
       <c r="E821" s="48" t="s">
@@ -34766,10 +34774,10 @@
         <v>3</v>
       </c>
       <c r="G821" s="39" t="s">
-        <v>2581</v>
+        <v>2577</v>
       </c>
       <c r="H821" s="39" t="s">
-        <v>2565</v>
+        <v>2561</v>
       </c>
       <c r="I821" s="49"/>
     </row>
@@ -34781,7 +34789,7 @@
         <v>2158</v>
       </c>
       <c r="C822" s="41" t="s">
-        <v>2631</v>
+        <v>2627</v>
       </c>
       <c r="D822" s="48"/>
       <c r="E822" s="48" t="s">
@@ -34831,7 +34839,7 @@
         <v>2159</v>
       </c>
       <c r="C824" s="41" t="s">
-        <v>2633</v>
+        <v>2629</v>
       </c>
       <c r="D824" s="48"/>
       <c r="E824" s="48" t="s">
@@ -34844,7 +34852,7 @@
         <v>15</v>
       </c>
       <c r="H824" s="39" t="s">
-        <v>2570</v>
+        <v>2566</v>
       </c>
       <c r="I824" s="49"/>
     </row>
@@ -34866,7 +34874,7 @@
         <v>3</v>
       </c>
       <c r="G825" s="39" t="s">
-        <v>2581</v>
+        <v>2577</v>
       </c>
       <c r="H825" s="48" t="s">
         <v>18</v>
@@ -34888,7 +34896,7 @@
         <v>19</v>
       </c>
       <c r="F826" s="39" t="s">
-        <v>2624</v>
+        <v>2620</v>
       </c>
       <c r="G826" s="48" t="s">
         <v>15</v>
@@ -34913,7 +34921,7 @@
         <v>19</v>
       </c>
       <c r="F827" s="39" t="s">
-        <v>2624</v>
+        <v>2620</v>
       </c>
       <c r="G827" s="48" t="s">
         <v>15</v>
@@ -34931,7 +34939,7 @@
         <v>2188</v>
       </c>
       <c r="C828" s="41" t="s">
-        <v>2635</v>
+        <v>2631</v>
       </c>
       <c r="D828" s="48"/>
       <c r="E828" s="48" t="s">
@@ -34944,7 +34952,7 @@
         <v>15</v>
       </c>
       <c r="H828" s="39" t="s">
-        <v>2570</v>
+        <v>2566</v>
       </c>
       <c r="I828" s="49"/>
     </row>
@@ -34956,7 +34964,7 @@
         <v>2188</v>
       </c>
       <c r="C829" s="41" t="s">
-        <v>2634</v>
+        <v>2630</v>
       </c>
       <c r="D829" s="48"/>
       <c r="E829" s="48" t="s">
@@ -34969,7 +34977,7 @@
         <v>15</v>
       </c>
       <c r="H829" s="39" t="s">
-        <v>2570</v>
+        <v>2566</v>
       </c>
       <c r="I829" s="49"/>
     </row>
@@ -34981,7 +34989,7 @@
         <v>2188</v>
       </c>
       <c r="C830" s="41" t="s">
-        <v>2625</v>
+        <v>2621</v>
       </c>
       <c r="D830" s="48"/>
       <c r="E830" s="48" t="s">
@@ -35031,7 +35039,7 @@
         <v>2188</v>
       </c>
       <c r="C832" s="41" t="s">
-        <v>2636</v>
+        <v>2632</v>
       </c>
       <c r="D832" s="48"/>
       <c r="E832" s="48" t="s">
@@ -35056,7 +35064,7 @@
         <v>2188</v>
       </c>
       <c r="C833" s="41" t="s">
-        <v>2668</v>
+        <v>2664</v>
       </c>
       <c r="D833" s="48"/>
       <c r="E833" s="48" t="s">
@@ -35069,7 +35077,7 @@
         <v>15</v>
       </c>
       <c r="H833" s="39" t="s">
-        <v>2564</v>
+        <v>2560</v>
       </c>
       <c r="I833" s="49"/>
     </row>
@@ -35088,7 +35096,7 @@
         <v>19</v>
       </c>
       <c r="F834" s="39" t="s">
-        <v>2624</v>
+        <v>2620</v>
       </c>
       <c r="G834" s="48" t="s">
         <v>15</v>
@@ -35113,7 +35121,7 @@
         <v>19</v>
       </c>
       <c r="F835" s="39" t="s">
-        <v>2624</v>
+        <v>2620</v>
       </c>
       <c r="G835" s="48" t="s">
         <v>15</v>
@@ -35138,13 +35146,13 @@
         <v>19</v>
       </c>
       <c r="F836" s="39" t="s">
-        <v>2624</v>
+        <v>2620</v>
       </c>
       <c r="G836" s="48" t="s">
         <v>15</v>
       </c>
       <c r="H836" s="39" t="s">
-        <v>2565</v>
+        <v>2561</v>
       </c>
       <c r="I836" s="49"/>
     </row>
@@ -35188,13 +35196,13 @@
         <v>19</v>
       </c>
       <c r="F838" s="39" t="s">
-        <v>2624</v>
+        <v>2620</v>
       </c>
       <c r="G838" s="48" t="s">
         <v>15</v>
       </c>
       <c r="H838" s="39" t="s">
-        <v>2565</v>
+        <v>2561</v>
       </c>
       <c r="I838" s="49"/>
     </row>
@@ -35213,7 +35221,7 @@
         <v>19</v>
       </c>
       <c r="F839" s="39" t="s">
-        <v>2624</v>
+        <v>2620</v>
       </c>
       <c r="G839" s="48" t="s">
         <v>15</v>
@@ -35238,13 +35246,13 @@
         <v>19</v>
       </c>
       <c r="F840" s="39" t="s">
-        <v>2624</v>
+        <v>2620</v>
       </c>
       <c r="G840" s="48" t="s">
         <v>15</v>
       </c>
       <c r="H840" s="39" t="s">
-        <v>2565</v>
+        <v>2561</v>
       </c>
       <c r="I840" s="49"/>
     </row>
@@ -35263,7 +35271,7 @@
         <v>19</v>
       </c>
       <c r="F841" s="39" t="s">
-        <v>2624</v>
+        <v>2620</v>
       </c>
       <c r="G841" s="48" t="s">
         <v>15</v>
@@ -35288,13 +35296,13 @@
         <v>19</v>
       </c>
       <c r="F842" s="39" t="s">
-        <v>2624</v>
+        <v>2620</v>
       </c>
       <c r="G842" s="48" t="s">
         <v>15</v>
       </c>
       <c r="H842" s="39" t="s">
-        <v>2565</v>
+        <v>2561</v>
       </c>
       <c r="I842" s="49"/>
     </row>
@@ -35313,7 +35321,7 @@
         <v>19</v>
       </c>
       <c r="F843" s="39" t="s">
-        <v>2624</v>
+        <v>2620</v>
       </c>
       <c r="G843" s="48" t="s">
         <v>15</v>
@@ -35338,13 +35346,13 @@
         <v>19</v>
       </c>
       <c r="F844" s="39" t="s">
-        <v>2624</v>
+        <v>2620</v>
       </c>
       <c r="G844" s="48" t="s">
         <v>15</v>
       </c>
       <c r="H844" s="39" t="s">
-        <v>2565</v>
+        <v>2561</v>
       </c>
       <c r="I844" s="49"/>
     </row>
@@ -35363,7 +35371,7 @@
         <v>19</v>
       </c>
       <c r="F845" s="39" t="s">
-        <v>2624</v>
+        <v>2620</v>
       </c>
       <c r="G845" s="48" t="s">
         <v>15</v>
@@ -35381,7 +35389,7 @@
         <v>2203</v>
       </c>
       <c r="C846" s="41" t="s">
-        <v>2638</v>
+        <v>2634</v>
       </c>
       <c r="D846" s="48"/>
       <c r="E846" s="48" t="s">
@@ -35394,7 +35402,7 @@
         <v>15</v>
       </c>
       <c r="H846" s="39" t="s">
-        <v>2570</v>
+        <v>2566</v>
       </c>
       <c r="I846" s="49"/>
     </row>
@@ -35406,7 +35414,7 @@
         <v>2203</v>
       </c>
       <c r="C847" s="41" t="s">
-        <v>2637</v>
+        <v>2633</v>
       </c>
       <c r="D847" s="48"/>
       <c r="E847" s="48" t="s">
@@ -35456,7 +35464,7 @@
         <v>2203</v>
       </c>
       <c r="C849" s="41" t="s">
-        <v>2639</v>
+        <v>2635</v>
       </c>
       <c r="D849" s="48"/>
       <c r="E849" s="48" t="s">
@@ -35481,7 +35489,7 @@
         <v>2203</v>
       </c>
       <c r="C850" s="41" t="s">
-        <v>2669</v>
+        <v>2665</v>
       </c>
       <c r="D850" s="48"/>
       <c r="E850" s="48" t="s">
@@ -35494,7 +35502,7 @@
         <v>15</v>
       </c>
       <c r="H850" s="39" t="s">
-        <v>2564</v>
+        <v>2560</v>
       </c>
       <c r="I850" s="49"/>
     </row>
@@ -35516,7 +35524,7 @@
         <v>3</v>
       </c>
       <c r="G851" s="39" t="s">
-        <v>2581</v>
+        <v>2577</v>
       </c>
       <c r="H851" s="48" t="s">
         <v>18</v>
@@ -35531,7 +35539,7 @@
         <v>2055</v>
       </c>
       <c r="C852" s="41" t="s">
-        <v>2640</v>
+        <v>2636</v>
       </c>
       <c r="D852" s="48"/>
       <c r="E852" s="48" t="s">
@@ -35581,7 +35589,7 @@
         <v>2055</v>
       </c>
       <c r="C854" s="41" t="s">
-        <v>2641</v>
+        <v>2637</v>
       </c>
       <c r="D854" s="48"/>
       <c r="E854" s="48" t="s">
@@ -35606,7 +35614,7 @@
         <v>2055</v>
       </c>
       <c r="C855" s="41" t="s">
-        <v>2655</v>
+        <v>2651</v>
       </c>
       <c r="D855" s="48"/>
       <c r="E855" s="48" t="s">
@@ -35619,7 +35627,7 @@
         <v>15</v>
       </c>
       <c r="H855" s="39" t="s">
-        <v>2564</v>
+        <v>2560</v>
       </c>
       <c r="I855" s="49"/>
     </row>
@@ -35631,7 +35639,7 @@
         <v>2055</v>
       </c>
       <c r="C856" s="41" t="s">
-        <v>2642</v>
+        <v>2638</v>
       </c>
       <c r="D856" s="48"/>
       <c r="E856" s="48" t="s">
@@ -35656,7 +35664,7 @@
         <v>2055</v>
       </c>
       <c r="C857" s="41" t="s">
-        <v>2654</v>
+        <v>2650</v>
       </c>
       <c r="D857" s="48"/>
       <c r="E857" s="48" t="s">
@@ -35669,7 +35677,7 @@
         <v>15</v>
       </c>
       <c r="H857" s="39" t="s">
-        <v>2564</v>
+        <v>2560</v>
       </c>
       <c r="I857" s="49"/>
     </row>
@@ -35681,7 +35689,7 @@
         <v>2055</v>
       </c>
       <c r="C858" s="41" t="s">
-        <v>2643</v>
+        <v>2639</v>
       </c>
       <c r="D858" s="48"/>
       <c r="E858" s="48" t="s">
@@ -35706,7 +35714,7 @@
         <v>2055</v>
       </c>
       <c r="C859" s="41" t="s">
-        <v>2662</v>
+        <v>2658</v>
       </c>
       <c r="D859" s="48"/>
       <c r="E859" s="48" t="s">
@@ -35719,7 +35727,7 @@
         <v>15</v>
       </c>
       <c r="H859" s="39" t="s">
-        <v>2564</v>
+        <v>2560</v>
       </c>
       <c r="I859" s="49"/>
     </row>
@@ -35731,7 +35739,7 @@
         <v>2055</v>
       </c>
       <c r="C860" s="41" t="s">
-        <v>2644</v>
+        <v>2640</v>
       </c>
       <c r="D860" s="48"/>
       <c r="E860" s="48" t="s">
@@ -35756,7 +35764,7 @@
         <v>2055</v>
       </c>
       <c r="C861" s="41" t="s">
-        <v>2663</v>
+        <v>2659</v>
       </c>
       <c r="D861" s="48"/>
       <c r="E861" s="48" t="s">
@@ -35769,7 +35777,7 @@
         <v>15</v>
       </c>
       <c r="H861" s="39" t="s">
-        <v>2564</v>
+        <v>2560</v>
       </c>
       <c r="I861" s="49"/>
     </row>
@@ -35781,7 +35789,7 @@
         <v>2055</v>
       </c>
       <c r="C862" s="41" t="s">
-        <v>2645</v>
+        <v>2641</v>
       </c>
       <c r="D862" s="48"/>
       <c r="E862" s="48" t="s">
@@ -35806,7 +35814,7 @@
         <v>2055</v>
       </c>
       <c r="C863" s="41" t="s">
-        <v>2664</v>
+        <v>2660</v>
       </c>
       <c r="D863" s="48"/>
       <c r="E863" s="48" t="s">
@@ -35819,7 +35827,7 @@
         <v>15</v>
       </c>
       <c r="H863" s="39" t="s">
-        <v>2564</v>
+        <v>2560</v>
       </c>
       <c r="I863" s="49"/>
     </row>
@@ -35831,7 +35839,7 @@
         <v>2055</v>
       </c>
       <c r="C864" s="41" t="s">
-        <v>2646</v>
+        <v>2642</v>
       </c>
       <c r="D864" s="48"/>
       <c r="E864" s="48" t="s">
@@ -35856,7 +35864,7 @@
         <v>2055</v>
       </c>
       <c r="C865" s="41" t="s">
-        <v>2665</v>
+        <v>2661</v>
       </c>
       <c r="D865" s="48"/>
       <c r="E865" s="48" t="s">
@@ -35869,7 +35877,7 @@
         <v>15</v>
       </c>
       <c r="H865" s="39" t="s">
-        <v>2564</v>
+        <v>2560</v>
       </c>
       <c r="I865" s="49"/>
     </row>
@@ -35881,7 +35889,7 @@
         <v>2055</v>
       </c>
       <c r="C866" s="41" t="s">
-        <v>2647</v>
+        <v>2643</v>
       </c>
       <c r="D866" s="48"/>
       <c r="E866" s="48" t="s">
@@ -35919,7 +35927,7 @@
         <v>15</v>
       </c>
       <c r="H867" s="39" t="s">
-        <v>2564</v>
+        <v>2560</v>
       </c>
       <c r="I867" s="49"/>
     </row>
@@ -35931,7 +35939,7 @@
         <v>2055</v>
       </c>
       <c r="C868" s="41" t="s">
-        <v>2648</v>
+        <v>2644</v>
       </c>
       <c r="D868" s="48"/>
       <c r="E868" s="48" t="s">
@@ -35950,7 +35958,7 @@
     </row>
     <row r="869" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A869" s="39" t="s">
-        <v>2657</v>
+        <v>2653</v>
       </c>
       <c r="B869" s="50" t="s">
         <v>2055</v>
@@ -35969,22 +35977,22 @@
         <v>15</v>
       </c>
       <c r="H869" s="39" t="s">
-        <v>2564</v>
+        <v>2560</v>
       </c>
       <c r="I869" s="41"/>
     </row>
     <row r="870" spans="1:9" s="37" customFormat="1">
       <c r="A870" s="39" t="s">
-        <v>2658</v>
+        <v>2654</v>
       </c>
       <c r="B870" s="50" t="s">
         <v>2055</v>
       </c>
       <c r="C870" s="41" t="s">
-        <v>2660</v>
+        <v>2656</v>
       </c>
       <c r="D870" s="39" t="s">
-        <v>2667</v>
+        <v>2663</v>
       </c>
       <c r="E870" s="48" t="s">
         <v>19</v>
@@ -35996,22 +36004,22 @@
         <v>15</v>
       </c>
       <c r="H870" s="39" t="s">
-        <v>2564</v>
+        <v>2560</v>
       </c>
       <c r="I870" s="41"/>
     </row>
     <row r="871" spans="1:9" s="37" customFormat="1">
       <c r="A871" s="39" t="s">
-        <v>2659</v>
+        <v>2655</v>
       </c>
       <c r="B871" s="50" t="s">
         <v>2055</v>
       </c>
       <c r="C871" s="41" t="s">
-        <v>2661</v>
+        <v>2657</v>
       </c>
       <c r="D871" s="39" t="s">
-        <v>2667</v>
+        <v>2663</v>
       </c>
       <c r="E871" s="48" t="s">
         <v>19</v>
@@ -36023,7 +36031,7 @@
         <v>15</v>
       </c>
       <c r="H871" s="39" t="s">
-        <v>2564</v>
+        <v>2560</v>
       </c>
       <c r="I871" s="49"/>
     </row>
@@ -36035,7 +36043,7 @@
         <v>2055</v>
       </c>
       <c r="C872" s="41" t="s">
-        <v>2649</v>
+        <v>2645</v>
       </c>
       <c r="D872" s="48"/>
       <c r="E872" s="48" t="s">
@@ -36060,7 +36068,7 @@
         <v>2055</v>
       </c>
       <c r="C873" s="41" t="s">
-        <v>2656</v>
+        <v>2652</v>
       </c>
       <c r="D873" s="48"/>
       <c r="E873" s="48" t="s">
@@ -36073,7 +36081,7 @@
         <v>15</v>
       </c>
       <c r="H873" s="39" t="s">
-        <v>2564</v>
+        <v>2560</v>
       </c>
       <c r="I873" s="49"/>
     </row>
@@ -36120,7 +36128,7 @@
         <v>3</v>
       </c>
       <c r="G875" s="39" t="s">
-        <v>2581</v>
+        <v>2577</v>
       </c>
       <c r="H875" s="39" t="s">
         <v>18</v>
@@ -36145,7 +36153,7 @@
         <v>3</v>
       </c>
       <c r="G876" s="39" t="s">
-        <v>2581</v>
+        <v>2577</v>
       </c>
       <c r="H876" s="39" t="s">
         <v>18</v>
@@ -36160,7 +36168,7 @@
         <v>2243</v>
       </c>
       <c r="C877" s="41" t="s">
-        <v>2650</v>
+        <v>2646</v>
       </c>
       <c r="D877" s="39"/>
       <c r="E877" s="39" t="s">
@@ -36210,7 +36218,7 @@
         <v>2243</v>
       </c>
       <c r="C879" s="41" t="s">
-        <v>2666</v>
+        <v>2662</v>
       </c>
       <c r="D879" s="39"/>
       <c r="E879" s="39" t="s">
@@ -36223,7 +36231,7 @@
         <v>15</v>
       </c>
       <c r="H879" s="39" t="s">
-        <v>2564</v>
+        <v>2560</v>
       </c>
       <c r="I879" s="41"/>
     </row>
@@ -36235,7 +36243,7 @@
         <v>2243</v>
       </c>
       <c r="C880" s="41" t="s">
-        <v>2670</v>
+        <v>2666</v>
       </c>
       <c r="D880" s="39"/>
       <c r="E880" s="39" t="s">
@@ -36248,7 +36256,7 @@
         <v>15</v>
       </c>
       <c r="H880" s="39" t="s">
-        <v>2564</v>
+        <v>2560</v>
       </c>
       <c r="I880" s="41"/>
     </row>
@@ -36729,7 +36737,7 @@
         <v>15</v>
       </c>
       <c r="H899" s="39" t="s">
-        <v>2564</v>
+        <v>2560</v>
       </c>
       <c r="I899" s="41"/>
     </row>
@@ -36782,7 +36790,7 @@
         <v>17</v>
       </c>
       <c r="I901" s="41" t="s">
-        <v>2536</v>
+        <v>2532</v>
       </c>
     </row>
     <row r="902" spans="1:9" ht="90">
@@ -39141,7 +39149,7 @@
     </row>
     <row r="996" spans="1:9" s="37" customFormat="1" ht="30">
       <c r="A996" s="39" t="s">
-        <v>2614</v>
+        <v>2610</v>
       </c>
       <c r="B996" s="40" t="s">
         <v>2248</v>
@@ -39160,7 +39168,7 @@
         <v>15</v>
       </c>
       <c r="H996" s="39" t="s">
-        <v>2565</v>
+        <v>2561</v>
       </c>
       <c r="I996" s="49"/>
     </row>
@@ -39650,7 +39658,7 @@
         <v>15</v>
       </c>
       <c r="H1014" s="39" t="s">
-        <v>2565</v>
+        <v>2561</v>
       </c>
       <c r="I1014" s="41"/>
     </row>
@@ -39662,7 +39670,7 @@
         <v>8</v>
       </c>
       <c r="C1015" s="41" t="s">
-        <v>2617</v>
+        <v>2613</v>
       </c>
       <c r="D1015" s="39" t="s">
         <v>1863</v>
@@ -39677,7 +39685,7 @@
         <v>15</v>
       </c>
       <c r="H1015" s="39" t="s">
-        <v>2565</v>
+        <v>2561</v>
       </c>
       <c r="I1015" s="41"/>
     </row>
@@ -39766,7 +39774,7 @@
     </row>
     <row r="1019" spans="1:9" ht="45">
       <c r="A1019" s="39" t="s">
-        <v>2674</v>
+        <v>2670</v>
       </c>
       <c r="B1019" s="43">
         <v>8</v>
@@ -39822,7 +39830,7 @@
     </row>
     <row r="1021" spans="1:9" ht="45">
       <c r="A1021" s="39" t="s">
-        <v>2675</v>
+        <v>2671</v>
       </c>
       <c r="B1021" s="43">
         <v>8</v>
@@ -39884,7 +39892,7 @@
         <v>893</v>
       </c>
       <c r="C1023" s="41" t="s">
-        <v>2562</v>
+        <v>2558</v>
       </c>
       <c r="D1023" s="39" t="s">
         <v>1926</v>
@@ -39913,10 +39921,10 @@
         <v>8</v>
       </c>
       <c r="C1024" s="41" t="s">
-        <v>2428</v>
+        <v>2427</v>
       </c>
       <c r="D1024" s="39" t="s">
-        <v>2427</v>
+        <v>2426</v>
       </c>
       <c r="E1024" s="48" t="s">
         <v>22</v>
@@ -39934,16 +39942,16 @@
     </row>
     <row r="1025" spans="1:9" ht="45">
       <c r="A1025" s="39" t="s">
-        <v>2426</v>
+        <v>2678</v>
       </c>
       <c r="B1025" s="43">
         <v>8</v>
       </c>
       <c r="C1025" s="41" t="s">
-        <v>2429</v>
+        <v>2677</v>
       </c>
       <c r="D1025" s="39" t="s">
-        <v>2427</v>
+        <v>2426</v>
       </c>
       <c r="E1025" s="48" t="s">
         <v>22</v>
@@ -39969,7 +39977,7 @@
         <v>893</v>
       </c>
       <c r="C1026" s="41" t="s">
-        <v>2433</v>
+        <v>2432</v>
       </c>
       <c r="D1026" s="39" t="s">
         <v>1529</v>
@@ -39998,7 +40006,7 @@
         <v>893</v>
       </c>
       <c r="C1027" s="41" t="s">
-        <v>2432</v>
+        <v>2431</v>
       </c>
       <c r="D1027" s="39" t="s">
         <v>1529</v>
@@ -40025,7 +40033,7 @@
         <v>893</v>
       </c>
       <c r="C1028" s="41" t="s">
-        <v>2431</v>
+        <v>2430</v>
       </c>
       <c r="D1028" s="39" t="s">
         <v>1530</v>
@@ -40081,7 +40089,7 @@
         <v>893</v>
       </c>
       <c r="C1030" s="41" t="s">
-        <v>2434</v>
+        <v>2433</v>
       </c>
       <c r="D1030" s="39" t="s">
         <v>1531</v>
@@ -40108,7 +40116,7 @@
         <v>893</v>
       </c>
       <c r="C1031" s="41" t="s">
-        <v>2435</v>
+        <v>2434</v>
       </c>
       <c r="D1031" s="39" t="s">
         <v>1531</v>
@@ -40131,16 +40139,16 @@
     </row>
     <row r="1032" spans="1:9" ht="45">
       <c r="A1032" s="39" t="s">
-        <v>2436</v>
+        <v>2435</v>
       </c>
       <c r="B1032" s="43">
         <v>8</v>
       </c>
       <c r="C1032" s="41" t="s">
-        <v>2474</v>
+        <v>2680</v>
       </c>
       <c r="D1032" s="39" t="s">
-        <v>2440</v>
+        <v>2439</v>
       </c>
       <c r="E1032" s="48" t="s">
         <v>22</v>
@@ -40160,16 +40168,16 @@
     </row>
     <row r="1033" spans="1:9" ht="30">
       <c r="A1033" s="39" t="s">
-        <v>2437</v>
+        <v>2436</v>
       </c>
       <c r="B1033" s="43">
         <v>8</v>
       </c>
       <c r="C1033" s="41" t="s">
-        <v>2438</v>
+        <v>2437</v>
       </c>
       <c r="D1033" s="39" t="s">
-        <v>2440</v>
+        <v>2439</v>
       </c>
       <c r="E1033" s="48" t="s">
         <v>22</v>
@@ -40187,16 +40195,16 @@
     </row>
     <row r="1034" spans="1:9" ht="30">
       <c r="A1034" s="39" t="s">
-        <v>2608</v>
+        <v>2604</v>
       </c>
       <c r="B1034" s="43">
         <v>8</v>
       </c>
       <c r="C1034" s="41" t="s">
-        <v>2609</v>
+        <v>2605</v>
       </c>
       <c r="D1034" s="39" t="s">
-        <v>2476</v>
+        <v>2472</v>
       </c>
       <c r="E1034" s="48" t="s">
         <v>22</v>
@@ -40214,16 +40222,16 @@
     </row>
     <row r="1035" spans="1:9" s="37" customFormat="1" ht="45">
       <c r="A1035" s="39" t="s">
-        <v>2561</v>
+        <v>2557</v>
       </c>
       <c r="B1035" s="43">
         <v>8</v>
       </c>
       <c r="C1035" s="41" t="s">
-        <v>2560</v>
+        <v>2556</v>
       </c>
       <c r="D1035" s="39" t="s">
-        <v>2476</v>
+        <v>2472</v>
       </c>
       <c r="E1035" s="48" t="s">
         <v>22</v>
@@ -40249,7 +40257,7 @@
         <v>893</v>
       </c>
       <c r="C1036" s="41" t="s">
-        <v>2441</v>
+        <v>2440</v>
       </c>
       <c r="D1036" s="39" t="s">
         <v>1532</v>
@@ -40276,7 +40284,7 @@
         <v>893</v>
       </c>
       <c r="C1037" s="41" t="s">
-        <v>2477</v>
+        <v>2473</v>
       </c>
       <c r="D1037" s="39" t="s">
         <v>1532</v>
@@ -40305,7 +40313,7 @@
         <v>893</v>
       </c>
       <c r="C1038" s="41" t="s">
-        <v>2442</v>
+        <v>2441</v>
       </c>
       <c r="D1038" s="39" t="s">
         <v>1533</v>
@@ -40332,7 +40340,7 @@
         <v>893</v>
       </c>
       <c r="C1039" s="41" t="s">
-        <v>2478</v>
+        <v>2474</v>
       </c>
       <c r="D1039" s="39" t="s">
         <v>1533</v>
@@ -40361,7 +40369,7 @@
         <v>893</v>
       </c>
       <c r="C1040" s="41" t="s">
-        <v>2443</v>
+        <v>2442</v>
       </c>
       <c r="D1040" s="39" t="s">
         <v>1534</v>
@@ -40388,7 +40396,7 @@
         <v>893</v>
       </c>
       <c r="C1041" s="41" t="s">
-        <v>2479</v>
+        <v>2475</v>
       </c>
       <c r="D1041" s="39" t="s">
         <v>1534</v>
@@ -40417,7 +40425,7 @@
         <v>893</v>
       </c>
       <c r="C1042" s="41" t="s">
-        <v>2444</v>
+        <v>2443</v>
       </c>
       <c r="D1042" s="39" t="s">
         <v>1535</v>
@@ -40444,7 +40452,7 @@
         <v>893</v>
       </c>
       <c r="C1043" s="41" t="s">
-        <v>2480</v>
+        <v>2476</v>
       </c>
       <c r="D1043" s="39" t="s">
         <v>1535</v>
@@ -40473,7 +40481,7 @@
         <v>893</v>
       </c>
       <c r="C1044" s="41" t="s">
-        <v>2445</v>
+        <v>2444</v>
       </c>
       <c r="D1044" s="39" t="s">
         <v>1536</v>
@@ -40500,7 +40508,7 @@
         <v>893</v>
       </c>
       <c r="C1045" s="41" t="s">
-        <v>2481</v>
+        <v>2477</v>
       </c>
       <c r="D1045" s="39" t="s">
         <v>1536</v>
@@ -40529,7 +40537,7 @@
         <v>893</v>
       </c>
       <c r="C1046" s="41" t="s">
-        <v>2446</v>
+        <v>2445</v>
       </c>
       <c r="D1046" s="39" t="s">
         <v>1537</v>
@@ -40556,7 +40564,7 @@
         <v>893</v>
       </c>
       <c r="C1047" s="41" t="s">
-        <v>2482</v>
+        <v>2478</v>
       </c>
       <c r="D1047" s="39" t="s">
         <v>1537</v>
@@ -40585,7 +40593,7 @@
         <v>893</v>
       </c>
       <c r="C1048" s="41" t="s">
-        <v>2447</v>
+        <v>2446</v>
       </c>
       <c r="D1048" s="39" t="s">
         <v>1538</v>
@@ -40612,7 +40620,7 @@
         <v>893</v>
       </c>
       <c r="C1049" s="41" t="s">
-        <v>2483</v>
+        <v>2479</v>
       </c>
       <c r="D1049" s="42" t="s">
         <v>1538</v>
@@ -40639,7 +40647,7 @@
         <v>893</v>
       </c>
       <c r="C1050" s="41" t="s">
-        <v>2448</v>
+        <v>2447</v>
       </c>
       <c r="D1050" s="39" t="s">
         <v>1539</v>
@@ -40666,7 +40674,7 @@
         <v>893</v>
       </c>
       <c r="C1051" s="41" t="s">
-        <v>2484</v>
+        <v>2480</v>
       </c>
       <c r="D1051" s="42" t="s">
         <v>1539</v>
@@ -40693,7 +40701,7 @@
         <v>893</v>
       </c>
       <c r="C1052" s="41" t="s">
-        <v>2449</v>
+        <v>2448</v>
       </c>
       <c r="D1052" s="39" t="s">
         <v>1540</v>
@@ -40720,7 +40728,7 @@
         <v>893</v>
       </c>
       <c r="C1053" s="41" t="s">
-        <v>2679</v>
+        <v>2675</v>
       </c>
       <c r="D1053" s="39" t="s">
         <v>1540</v>
@@ -40749,7 +40757,7 @@
         <v>893</v>
       </c>
       <c r="C1054" s="41" t="s">
-        <v>2450</v>
+        <v>2449</v>
       </c>
       <c r="D1054" s="39" t="s">
         <v>1541</v>
@@ -40805,7 +40813,7 @@
         <v>893</v>
       </c>
       <c r="C1056" s="41" t="s">
-        <v>2451</v>
+        <v>2450</v>
       </c>
       <c r="D1056" s="39" t="s">
         <v>1867</v>
@@ -40832,7 +40840,7 @@
         <v>893</v>
       </c>
       <c r="C1057" s="41" t="s">
-        <v>2610</v>
+        <v>2606</v>
       </c>
       <c r="D1057" s="39" t="s">
         <v>1867</v>
@@ -40859,7 +40867,7 @@
         <v>893</v>
       </c>
       <c r="C1058" s="41" t="s">
-        <v>2452</v>
+        <v>2451</v>
       </c>
       <c r="D1058" s="39" t="s">
         <v>1542</v>
@@ -40915,7 +40923,7 @@
         <v>893</v>
       </c>
       <c r="C1060" s="41" t="s">
-        <v>2453</v>
+        <v>2452</v>
       </c>
       <c r="D1060" s="39" t="s">
         <v>1543</v>
@@ -40971,7 +40979,7 @@
         <v>893</v>
       </c>
       <c r="C1062" s="41" t="s">
-        <v>2454</v>
+        <v>2453</v>
       </c>
       <c r="D1062" s="39" t="s">
         <v>1544</v>
@@ -41027,7 +41035,7 @@
         <v>893</v>
       </c>
       <c r="C1064" s="41" t="s">
-        <v>2455</v>
+        <v>2454</v>
       </c>
       <c r="D1064" s="39" t="s">
         <v>1545</v>
@@ -41083,7 +41091,7 @@
         <v>893</v>
       </c>
       <c r="C1066" s="41" t="s">
-        <v>2456</v>
+        <v>2455</v>
       </c>
       <c r="D1066" s="39" t="s">
         <v>1546</v>
@@ -41139,7 +41147,7 @@
         <v>893</v>
       </c>
       <c r="C1068" s="41" t="s">
-        <v>2457</v>
+        <v>2456</v>
       </c>
       <c r="D1068" s="39" t="s">
         <v>1868</v>
@@ -41195,7 +41203,7 @@
         <v>893</v>
       </c>
       <c r="C1070" s="41" t="s">
-        <v>2458</v>
+        <v>2457</v>
       </c>
       <c r="D1070" s="39" t="s">
         <v>1547</v>
@@ -41251,7 +41259,7 @@
         <v>8</v>
       </c>
       <c r="C1072" s="41" t="s">
-        <v>2459</v>
+        <v>2458</v>
       </c>
       <c r="D1072" s="39" t="s">
         <v>1869</v>
@@ -41301,13 +41309,13 @@
     </row>
     <row r="1074" spans="1:9" ht="45">
       <c r="A1074" s="39" t="s">
-        <v>2460</v>
+        <v>2459</v>
       </c>
       <c r="B1074" s="43">
         <v>8</v>
       </c>
       <c r="C1074" s="41" t="s">
-        <v>2462</v>
+        <v>2461</v>
       </c>
       <c r="D1074" s="39" t="s">
         <v>1916</v>
@@ -41328,13 +41336,13 @@
     </row>
     <row r="1075" spans="1:9" ht="45">
       <c r="A1075" s="39" t="s">
-        <v>2461</v>
+        <v>2460</v>
       </c>
       <c r="B1075" s="43">
         <v>8</v>
       </c>
       <c r="C1075" s="41" t="s">
-        <v>2429</v>
+        <v>2428</v>
       </c>
       <c r="D1075" s="39" t="s">
         <v>1916</v>
@@ -41363,7 +41371,7 @@
         <v>893</v>
       </c>
       <c r="C1076" s="41" t="s">
-        <v>2485</v>
+        <v>2481</v>
       </c>
       <c r="D1076" s="39" t="s">
         <v>1548</v>
@@ -41392,7 +41400,7 @@
         <v>893</v>
       </c>
       <c r="C1077" s="41" t="s">
-        <v>2486</v>
+        <v>2482</v>
       </c>
       <c r="D1077" s="39" t="s">
         <v>1548</v>
@@ -41419,7 +41427,7 @@
         <v>893</v>
       </c>
       <c r="C1078" s="41" t="s">
-        <v>2464</v>
+        <v>2463</v>
       </c>
       <c r="D1078" s="39" t="s">
         <v>1549</v>
@@ -41446,7 +41454,7 @@
         <v>893</v>
       </c>
       <c r="C1079" s="41" t="s">
-        <v>2487</v>
+        <v>2483</v>
       </c>
       <c r="D1079" s="39" t="s">
         <v>1549</v>
@@ -41475,7 +41483,7 @@
         <v>893</v>
       </c>
       <c r="C1080" s="41" t="s">
-        <v>2465</v>
+        <v>2464</v>
       </c>
       <c r="D1080" s="39" t="s">
         <v>1550</v>
@@ -41502,7 +41510,7 @@
         <v>893</v>
       </c>
       <c r="C1081" s="41" t="s">
-        <v>2488</v>
+        <v>2484</v>
       </c>
       <c r="D1081" s="39" t="s">
         <v>1550</v>
@@ -41525,16 +41533,16 @@
     </row>
     <row r="1082" spans="1:9" ht="60">
       <c r="A1082" s="39" t="s">
-        <v>2466</v>
+        <v>2679</v>
       </c>
       <c r="B1082" s="43">
         <v>8</v>
       </c>
       <c r="C1082" s="41" t="s">
-        <v>2468</v>
+        <v>2681</v>
       </c>
       <c r="D1082" s="39" t="s">
-        <v>2470</v>
+        <v>2467</v>
       </c>
       <c r="E1082" s="48" t="s">
         <v>22</v>
@@ -41554,7 +41562,7 @@
     </row>
     <row r="1083" spans="1:9" ht="30">
       <c r="A1083" s="39" t="s">
-        <v>2467</v>
+        <v>2465</v>
       </c>
       <c r="B1083" s="43">
         <v>8</v>
@@ -41563,7 +41571,7 @@
         <v>1914</v>
       </c>
       <c r="D1083" s="39" t="s">
-        <v>2470</v>
+        <v>2467</v>
       </c>
       <c r="E1083" s="48" t="s">
         <v>22</v>
@@ -41587,7 +41595,7 @@
         <v>893</v>
       </c>
       <c r="C1084" s="41" t="s">
-        <v>2471</v>
+        <v>2468</v>
       </c>
       <c r="D1084" s="39" t="s">
         <v>1551</v>
@@ -41614,7 +41622,7 @@
         <v>893</v>
       </c>
       <c r="C1085" s="41" t="s">
-        <v>2489</v>
+        <v>2485</v>
       </c>
       <c r="D1085" s="39" t="s">
         <v>1551</v>
@@ -41643,7 +41651,7 @@
         <v>893</v>
       </c>
       <c r="C1086" s="41" t="s">
-        <v>2472</v>
+        <v>2469</v>
       </c>
       <c r="D1086" s="39" t="s">
         <v>1552</v>
@@ -41670,7 +41678,7 @@
         <v>893</v>
       </c>
       <c r="C1087" s="41" t="s">
-        <v>2490</v>
+        <v>2486</v>
       </c>
       <c r="D1087" s="39" t="s">
         <v>1552</v>
@@ -41699,7 +41707,7 @@
         <v>893</v>
       </c>
       <c r="C1088" s="41" t="s">
-        <v>2473</v>
+        <v>2470</v>
       </c>
       <c r="D1088" s="39" t="s">
         <v>1553</v>
@@ -41726,7 +41734,7 @@
         <v>893</v>
       </c>
       <c r="C1089" s="41" t="s">
-        <v>2491</v>
+        <v>2487</v>
       </c>
       <c r="D1089" s="39" t="s">
         <v>1553</v>
@@ -41755,7 +41763,7 @@
         <v>893</v>
       </c>
       <c r="C1090" s="41" t="s">
-        <v>2492</v>
+        <v>2488</v>
       </c>
       <c r="D1090" s="39" t="s">
         <v>1554</v>
@@ -41782,7 +41790,7 @@
         <v>893</v>
       </c>
       <c r="C1091" s="41" t="s">
-        <v>2493</v>
+        <v>2489</v>
       </c>
       <c r="D1091" s="39" t="s">
         <v>1554</v>
@@ -41811,7 +41819,7 @@
         <v>893</v>
       </c>
       <c r="C1092" s="41" t="s">
-        <v>2494</v>
+        <v>2490</v>
       </c>
       <c r="D1092" s="39" t="s">
         <v>1555</v>
@@ -41838,7 +41846,7 @@
         <v>893</v>
       </c>
       <c r="C1093" s="41" t="s">
-        <v>2495</v>
+        <v>2491</v>
       </c>
       <c r="D1093" s="39" t="s">
         <v>1555</v>
@@ -41867,7 +41875,7 @@
         <v>893</v>
       </c>
       <c r="C1094" s="41" t="s">
-        <v>2496</v>
+        <v>2492</v>
       </c>
       <c r="D1094" s="39" t="s">
         <v>1556</v>
@@ -41923,7 +41931,7 @@
         <v>893</v>
       </c>
       <c r="C1096" s="41" t="s">
-        <v>2497</v>
+        <v>2493</v>
       </c>
       <c r="D1096" s="39" t="s">
         <v>1557</v>
@@ -41979,7 +41987,7 @@
         <v>893</v>
       </c>
       <c r="C1098" s="41" t="s">
-        <v>2498</v>
+        <v>2494</v>
       </c>
       <c r="D1098" s="39" t="s">
         <v>1558</v>
@@ -42035,7 +42043,7 @@
         <v>893</v>
       </c>
       <c r="C1100" s="41" t="s">
-        <v>2499</v>
+        <v>2495</v>
       </c>
       <c r="D1100" s="39" t="s">
         <v>1559</v>
@@ -42091,7 +42099,7 @@
         <v>893</v>
       </c>
       <c r="C1102" s="41" t="s">
-        <v>2500</v>
+        <v>2496</v>
       </c>
       <c r="D1102" s="39" t="s">
         <v>1560</v>
@@ -42147,7 +42155,7 @@
         <v>893</v>
       </c>
       <c r="C1104" s="41" t="s">
-        <v>2501</v>
+        <v>2497</v>
       </c>
       <c r="D1104" s="39" t="s">
         <v>1561</v>
@@ -42201,7 +42209,7 @@
         <v>893</v>
       </c>
       <c r="C1106" s="41" t="s">
-        <v>2502</v>
+        <v>2498</v>
       </c>
       <c r="D1106" s="39" t="s">
         <v>1562</v>
@@ -42255,7 +42263,7 @@
         <v>893</v>
       </c>
       <c r="C1108" s="41" t="s">
-        <v>2503</v>
+        <v>2499</v>
       </c>
       <c r="D1108" s="39" t="s">
         <v>1563</v>
@@ -42282,7 +42290,7 @@
         <v>893</v>
       </c>
       <c r="C1109" s="41" t="s">
-        <v>2504</v>
+        <v>2500</v>
       </c>
       <c r="D1109" s="39" t="s">
         <v>1563</v>
@@ -42311,7 +42319,7 @@
         <v>893</v>
       </c>
       <c r="C1110" s="41" t="s">
-        <v>2505</v>
+        <v>2501</v>
       </c>
       <c r="D1110" s="39" t="s">
         <v>1564</v>
@@ -42365,7 +42373,7 @@
         <v>893</v>
       </c>
       <c r="C1112" s="41" t="s">
-        <v>2506</v>
+        <v>2502</v>
       </c>
       <c r="D1112" s="39" t="s">
         <v>1870</v>
@@ -42421,7 +42429,7 @@
         <v>893</v>
       </c>
       <c r="C1114" s="41" t="s">
-        <v>2508</v>
+        <v>2504</v>
       </c>
       <c r="D1114" s="39" t="s">
         <v>1565</v>
@@ -42450,7 +42458,7 @@
         <v>893</v>
       </c>
       <c r="C1115" s="41" t="s">
-        <v>2507</v>
+        <v>2503</v>
       </c>
       <c r="D1115" s="39" t="s">
         <v>1566</v>
@@ -42504,7 +42512,7 @@
         <v>893</v>
       </c>
       <c r="C1117" s="41" t="s">
-        <v>2509</v>
+        <v>2505</v>
       </c>
       <c r="D1117" s="39" t="s">
         <v>1567</v>
@@ -42558,7 +42566,7 @@
         <v>893</v>
       </c>
       <c r="C1119" s="41" t="s">
-        <v>2510</v>
+        <v>2506</v>
       </c>
       <c r="D1119" s="39" t="s">
         <v>1568</v>
@@ -42612,7 +42620,7 @@
         <v>893</v>
       </c>
       <c r="C1121" s="41" t="s">
-        <v>2511</v>
+        <v>2507</v>
       </c>
       <c r="D1121" s="39" t="s">
         <v>1871</v>
@@ -42639,7 +42647,7 @@
         <v>893</v>
       </c>
       <c r="C1122" s="41" t="s">
-        <v>2599</v>
+        <v>2595</v>
       </c>
       <c r="D1122" s="39" t="s">
         <v>1871</v>
@@ -42654,10 +42662,10 @@
         <v>15</v>
       </c>
       <c r="H1122" s="39" t="s">
-        <v>2570</v>
+        <v>2566</v>
       </c>
       <c r="I1122" s="41" t="s">
-        <v>2600</v>
+        <v>2596</v>
       </c>
     </row>
     <row r="1123" spans="1:9" ht="45">
@@ -42668,7 +42676,7 @@
         <v>893</v>
       </c>
       <c r="C1123" s="41" t="s">
-        <v>2512</v>
+        <v>2508</v>
       </c>
       <c r="D1123" s="39" t="s">
         <v>1872</v>
@@ -42695,7 +42703,7 @@
         <v>893</v>
       </c>
       <c r="C1124" s="41" t="s">
-        <v>2601</v>
+        <v>2597</v>
       </c>
       <c r="D1124" s="39" t="s">
         <v>1872</v>
@@ -42710,10 +42718,10 @@
         <v>15</v>
       </c>
       <c r="H1124" s="39" t="s">
-        <v>2570</v>
+        <v>2566</v>
       </c>
       <c r="I1124" s="41" t="s">
-        <v>2600</v>
+        <v>2596</v>
       </c>
     </row>
     <row r="1125" spans="1:9" ht="30">
@@ -42724,7 +42732,7 @@
         <v>893</v>
       </c>
       <c r="C1125" s="41" t="s">
-        <v>2513</v>
+        <v>2509</v>
       </c>
       <c r="D1125" s="39" t="s">
         <v>1569</v>
@@ -42772,16 +42780,16 @@
     </row>
     <row r="1127" spans="1:9" ht="30">
       <c r="A1127" s="39" t="s">
-        <v>2514</v>
+        <v>2510</v>
       </c>
       <c r="B1127" s="43">
         <v>8</v>
       </c>
       <c r="C1127" s="41" t="s">
-        <v>2515</v>
+        <v>2511</v>
       </c>
       <c r="D1127" s="39" t="s">
-        <v>2517</v>
+        <v>2513</v>
       </c>
       <c r="E1127" s="48" t="s">
         <v>22</v>
@@ -42799,16 +42807,16 @@
     </row>
     <row r="1128" spans="1:9" ht="45">
       <c r="A1128" s="39" t="s">
-        <v>2677</v>
+        <v>2673</v>
       </c>
       <c r="B1128" s="43">
         <v>8</v>
       </c>
       <c r="C1128" s="41" t="s">
-        <v>2678</v>
+        <v>2674</v>
       </c>
       <c r="D1128" s="48" t="s">
-        <v>2517</v>
+        <v>2513</v>
       </c>
       <c r="E1128" s="48" t="s">
         <v>22</v>
@@ -42834,7 +42842,7 @@
         <v>893</v>
       </c>
       <c r="C1129" s="41" t="s">
-        <v>2518</v>
+        <v>2514</v>
       </c>
       <c r="D1129" s="39" t="s">
         <v>1570</v>
@@ -42888,7 +42896,7 @@
         <v>893</v>
       </c>
       <c r="C1131" s="41" t="s">
-        <v>2519</v>
+        <v>2515</v>
       </c>
       <c r="D1131" s="39" t="s">
         <v>1571</v>
@@ -42942,7 +42950,7 @@
         <v>893</v>
       </c>
       <c r="C1133" s="41" t="s">
-        <v>2520</v>
+        <v>2516</v>
       </c>
       <c r="D1133" s="39" t="s">
         <v>1572</v>
@@ -42990,16 +42998,16 @@
     </row>
     <row r="1135" spans="1:9" ht="60">
       <c r="A1135" s="39" t="s">
-        <v>2521</v>
+        <v>2517</v>
       </c>
       <c r="B1135" s="43">
         <v>8</v>
       </c>
       <c r="C1135" s="41" t="s">
-        <v>2522</v>
+        <v>2518</v>
       </c>
       <c r="D1135" s="39" t="s">
-        <v>2524</v>
+        <v>2520</v>
       </c>
       <c r="E1135" s="48" t="s">
         <v>22</v>
@@ -43017,16 +43025,16 @@
     </row>
     <row r="1136" spans="1:9" ht="45">
       <c r="A1136" s="39" t="s">
-        <v>2615</v>
+        <v>2611</v>
       </c>
       <c r="B1136" s="43">
         <v>8</v>
       </c>
       <c r="C1136" s="41" t="s">
-        <v>2523</v>
+        <v>2519</v>
       </c>
       <c r="D1136" s="39" t="s">
-        <v>2524</v>
+        <v>2520</v>
       </c>
       <c r="E1136" s="48" t="s">
         <v>22</v>
@@ -43052,7 +43060,7 @@
         <v>893</v>
       </c>
       <c r="C1137" s="41" t="s">
-        <v>2525</v>
+        <v>2521</v>
       </c>
       <c r="D1137" s="39" t="s">
         <v>1573</v>
@@ -43131,16 +43139,16 @@
     </row>
     <row r="1140" spans="1:9" ht="30">
       <c r="A1140" s="39" t="s">
-        <v>2528</v>
+        <v>2524</v>
       </c>
       <c r="B1140" s="43">
         <v>8</v>
       </c>
       <c r="C1140" s="41" t="s">
-        <v>2532</v>
+        <v>2528</v>
       </c>
       <c r="D1140" s="39" t="s">
-        <v>2538</v>
+        <v>2534</v>
       </c>
       <c r="E1140" s="48" t="s">
         <v>22</v>
@@ -43158,16 +43166,16 @@
     </row>
     <row r="1141" spans="1:9" s="37" customFormat="1" ht="45">
       <c r="A1141" s="39" t="s">
-        <v>2529</v>
+        <v>2525</v>
       </c>
       <c r="B1141" s="43">
         <v>8</v>
       </c>
       <c r="C1141" s="41" t="s">
-        <v>2620</v>
+        <v>2616</v>
       </c>
       <c r="D1141" s="39" t="s">
-        <v>2538</v>
+        <v>2534</v>
       </c>
       <c r="E1141" s="48" t="s">
         <v>22</v>
@@ -43187,16 +43195,16 @@
     </row>
     <row r="1142" spans="1:9" ht="45">
       <c r="A1142" s="39" t="s">
-        <v>2530</v>
+        <v>2526</v>
       </c>
       <c r="B1142" s="43">
         <v>8</v>
       </c>
       <c r="C1142" s="41" t="s">
+        <v>2529</v>
+      </c>
+      <c r="D1142" s="39" t="s">
         <v>2533</v>
-      </c>
-      <c r="D1142" s="39" t="s">
-        <v>2537</v>
       </c>
       <c r="E1142" s="48" t="s">
         <v>22</v>
@@ -43214,16 +43222,16 @@
     </row>
     <row r="1143" spans="1:9" ht="45">
       <c r="A1143" s="39" t="s">
-        <v>2531</v>
+        <v>2527</v>
       </c>
       <c r="B1143" s="43">
         <v>8</v>
       </c>
       <c r="C1143" s="41" t="s">
-        <v>2534</v>
+        <v>2530</v>
       </c>
       <c r="D1143" s="39" t="s">
-        <v>2537</v>
+        <v>2533</v>
       </c>
       <c r="E1143" s="48" t="s">
         <v>22</v>
@@ -43346,7 +43354,7 @@
         <v>802</v>
       </c>
       <c r="B1148" s="40" t="s">
-        <v>2539</v>
+        <v>2535</v>
       </c>
       <c r="C1148" s="41" t="s">
         <v>1456</v>
@@ -43371,7 +43379,7 @@
         <v>803</v>
       </c>
       <c r="B1149" s="40" t="s">
-        <v>2539</v>
+        <v>2535</v>
       </c>
       <c r="C1149" s="41" t="s">
         <v>1457</v>
@@ -43398,7 +43406,7 @@
         <v>804</v>
       </c>
       <c r="B1150" s="40" t="s">
-        <v>2539</v>
+        <v>2535</v>
       </c>
       <c r="C1150" s="41" t="s">
         <v>1458</v>
@@ -43425,7 +43433,7 @@
         <v>805</v>
       </c>
       <c r="B1151" s="40" t="s">
-        <v>2539</v>
+        <v>2535</v>
       </c>
       <c r="C1151" s="41" t="s">
         <v>1459</v>
@@ -43452,7 +43460,7 @@
         <v>806</v>
       </c>
       <c r="B1152" s="40" t="s">
-        <v>2539</v>
+        <v>2535</v>
       </c>
       <c r="C1152" s="41" t="s">
         <v>1460</v>
@@ -43479,7 +43487,7 @@
         <v>807</v>
       </c>
       <c r="B1153" s="40" t="s">
-        <v>2539</v>
+        <v>2535</v>
       </c>
       <c r="C1153" s="41" t="s">
         <v>1461</v>
@@ -43506,10 +43514,10 @@
         <v>808</v>
       </c>
       <c r="B1154" s="40" t="s">
-        <v>2539</v>
+        <v>2535</v>
       </c>
       <c r="C1154" s="41" t="s">
-        <v>2540</v>
+        <v>2536</v>
       </c>
       <c r="D1154" s="39"/>
       <c r="E1154" s="39" t="s">
@@ -43531,7 +43539,7 @@
         <v>809</v>
       </c>
       <c r="B1155" s="40" t="s">
-        <v>2542</v>
+        <v>2538</v>
       </c>
       <c r="C1155" s="41" t="s">
         <v>1462</v>
@@ -43556,7 +43564,7 @@
         <v>810</v>
       </c>
       <c r="B1156" s="40" t="s">
-        <v>2543</v>
+        <v>2539</v>
       </c>
       <c r="C1156" s="41" t="s">
         <v>1463</v>
@@ -43581,7 +43589,7 @@
         <v>811</v>
       </c>
       <c r="B1157" s="40" t="s">
-        <v>2544</v>
+        <v>2540</v>
       </c>
       <c r="C1157" s="41" t="s">
         <v>1464</v>
@@ -43608,7 +43616,7 @@
         <v>812</v>
       </c>
       <c r="B1158" s="40" t="s">
-        <v>2544</v>
+        <v>2540</v>
       </c>
       <c r="C1158" s="41" t="s">
         <v>1465</v>
@@ -43633,7 +43641,7 @@
         <v>1917</v>
       </c>
       <c r="B1159" s="40" t="s">
-        <v>2545</v>
+        <v>2541</v>
       </c>
       <c r="C1159" s="41" t="s">
         <v>1918</v>
@@ -43788,7 +43796,7 @@
         <v>864</v>
       </c>
       <c r="C1165" s="41" t="s">
-        <v>2546</v>
+        <v>2542</v>
       </c>
       <c r="D1165" s="39"/>
       <c r="E1165" s="39" t="s">
@@ -43935,7 +43943,7 @@
         <v>824</v>
       </c>
       <c r="B1171" s="40" t="s">
-        <v>2548</v>
+        <v>2544</v>
       </c>
       <c r="C1171" s="41" t="s">
         <v>1476</v>
@@ -43960,7 +43968,7 @@
         <v>825</v>
       </c>
       <c r="B1172" s="40" t="s">
-        <v>2549</v>
+        <v>2545</v>
       </c>
       <c r="C1172" s="41" t="s">
         <v>1477</v>
@@ -43985,7 +43993,7 @@
         <v>826</v>
       </c>
       <c r="B1173" s="40" t="s">
-        <v>2550</v>
+        <v>2546</v>
       </c>
       <c r="C1173" s="41" t="s">
         <v>1478</v>
@@ -44010,7 +44018,7 @@
         <v>827</v>
       </c>
       <c r="B1174" s="40" t="s">
-        <v>2551</v>
+        <v>2547</v>
       </c>
       <c r="C1174" s="41" t="s">
         <v>1479</v>
@@ -44035,7 +44043,7 @@
         <v>828</v>
       </c>
       <c r="B1175" s="40" t="s">
-        <v>2552</v>
+        <v>2548</v>
       </c>
       <c r="C1175" s="41" t="s">
         <v>1480</v>
@@ -44060,7 +44068,7 @@
         <v>829</v>
       </c>
       <c r="B1176" s="40" t="s">
-        <v>2553</v>
+        <v>2549</v>
       </c>
       <c r="C1176" s="41" t="s">
         <v>1481</v>
@@ -44085,7 +44093,7 @@
         <v>830</v>
       </c>
       <c r="B1177" s="40" t="s">
-        <v>2554</v>
+        <v>2550</v>
       </c>
       <c r="C1177" s="41" t="s">
         <v>1482</v>
@@ -44110,7 +44118,7 @@
         <v>831</v>
       </c>
       <c r="B1178" s="40" t="s">
-        <v>2554</v>
+        <v>2550</v>
       </c>
       <c r="C1178" s="41" t="s">
         <v>1483</v>
@@ -44135,7 +44143,7 @@
         <v>832</v>
       </c>
       <c r="B1179" s="40" t="s">
-        <v>2554</v>
+        <v>2550</v>
       </c>
       <c r="C1179" s="41" t="s">
         <v>1484</v>
@@ -44160,7 +44168,7 @@
         <v>833</v>
       </c>
       <c r="B1180" s="40" t="s">
-        <v>2554</v>
+        <v>2550</v>
       </c>
       <c r="C1180" s="41" t="s">
         <v>1485</v>
@@ -44210,7 +44218,7 @@
         <v>835</v>
       </c>
       <c r="B1182" s="40" t="s">
-        <v>2555</v>
+        <v>2551</v>
       </c>
       <c r="C1182" s="41" t="s">
         <v>1487</v>
@@ -44288,7 +44296,7 @@
         <v>893</v>
       </c>
       <c r="C1185" s="41" t="s">
-        <v>2541</v>
+        <v>2537</v>
       </c>
       <c r="D1185" s="39" t="s">
         <v>1574</v>
@@ -44315,7 +44323,7 @@
         <v>893</v>
       </c>
       <c r="C1186" s="41" t="s">
-        <v>2680</v>
+        <v>2676</v>
       </c>
       <c r="D1186" s="39" t="s">
         <v>1574</v>
@@ -44330,7 +44338,7 @@
         <v>15</v>
       </c>
       <c r="H1186" s="39" t="s">
-        <v>2564</v>
+        <v>2560</v>
       </c>
       <c r="I1186" s="41" t="s">
         <v>1610</v>
@@ -44400,7 +44408,7 @@
         <v>893</v>
       </c>
       <c r="C1189" s="41" t="s">
-        <v>2547</v>
+        <v>2543</v>
       </c>
       <c r="D1189" s="39" t="s">
         <v>1575</v>
@@ -44456,17 +44464,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B8:I8"/>
     <mergeCell ref="B18:I18"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B16:I16"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B8:I8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1050:I1050 A1117:I1117 A1119:I1119 A1125:I1125 A1129:I1129 A1131:I1131 A1133:I1133 A1137:I1143 E133:H133 E148:H148 E198:H198 E351:H351 E1030:I1030 E1036:I1048 E1080:I1080 E1092:I1092 E131:I132 E130:H130 E349:I350 E348:H348 E211:H212 E341:I347 E433:I460 E431:H432 E463:I469 E461:H462 E470:H470 E1154:H1154 E1144:I1153 E1029:H1029 E1031:H1035 E1079:H1079 E1081:H1083 E1091:H1091 E1093:H1093 E1101:H1101 C1049:E1049 C1051:E1051 C1116:E1116 C1118:E1118 C1120:E1120 C1126:E1128 C1130:E1130 C1132:E1132 E332:H334 E134:I147 A1026:D1048 E199:I208 E1028:I1028 E1026:H1027 E210:I210 E209:H209 E325:I331 E324:H324 E430:I430 E429:H429 E471:I484 E107:I129 E106:H106 I81 A278:I278 H279:I279 E336:H340 A81 A279 A335 E1078:I1078 A1076:I1077 A1144:D1190 E1071:H1071 E1072:I1075 A20:I80 A82:I86 E87:I105 E149:I197 A298:D334 E298:I323 A795:B795 D795:I795 A847:B847 D847:I847 A1022:B1025 D1022:I1025 A1052:D1075 E1052:I1070 E1084:I1090 E1094:I1100 E1102:I1109 A1078:D1109 A1110:I1110 I1112 C1111:E1111 H1111 A1112:H1114 A1115:I1115 H1120 A1121:A1124 C1121:H1124 C1134:H1136 A796:I846 A87:D277 E213:I277 A280:I297 A336:D484 E352:I428 A485:I794 A848:I869 A872:I1012 A870:C871 E870:I871 E1155:I1190">
@@ -46656,15 +46664,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -46713,6 +46712,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement/>
@@ -46720,14 +46728,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -46738,6 +46738,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>